<commit_message>
Sourced all the switches
</commit_message>
<xml_diff>
--- a/r2/bom/tr20-r2-alternative-sources.xlsx
+++ b/r2/bom/tr20-r2-alternative-sources.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="401">
   <si>
     <t xml:space="preserve">References</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Manufacturer</t>
   </si>
   <si>
-    <t xml:space="preserve">MPN Allnet</t>
+    <t xml:space="preserve">MPN</t>
   </si>
   <si>
     <t xml:space="preserve">Digikey</t>
@@ -631,10 +631,13 @@
     <t xml:space="preserve">10uH 1A</t>
   </si>
   <si>
-    <t xml:space="preserve">SXN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMNR5020-100MT</t>
+    <t xml:space="preserve">Taiyo Yuden </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRS4018T100MDGJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">587-2886-6-ND </t>
   </si>
   <si>
     <t xml:space="preserve">C135285</t>
@@ -736,6 +739,9 @@
     <t xml:space="preserve">Diodes Incorporated</t>
   </si>
   <si>
+    <t xml:space="preserve">DMG2305UX-13DIDKR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">C144153</t>
   </si>
   <si>
@@ -754,6 +760,9 @@
     <t xml:space="preserve">Micro Commercial Co</t>
   </si>
   <si>
+    <t xml:space="preserve">MMBT3904TPMSTR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">C77991</t>
   </si>
   <si>
@@ -769,6 +778,9 @@
     <t xml:space="preserve">Toshiba</t>
   </si>
   <si>
+    <t xml:space="preserve">SSM3K376RLFDKR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">C113202 </t>
   </si>
   <si>
@@ -784,6 +796,15 @@
     <t xml:space="preserve">0R</t>
   </si>
   <si>
+    <t xml:space="preserve">Yageo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-070RL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-0.0LRTR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">+/- 1%</t>
   </si>
   <si>
@@ -796,6 +817,12 @@
     <t xml:space="preserve">10R</t>
   </si>
   <si>
+    <t xml:space="preserve">RC0402FR-0710RL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-10.0LRTR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">+/- 5%</t>
   </si>
   <si>
@@ -805,6 +832,12 @@
     <t xml:space="preserve">10k</t>
   </si>
   <si>
+    <t xml:space="preserve">RC0402FR-0710KL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-10.0KLRTR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">+/- 10%</t>
   </si>
   <si>
@@ -814,25 +847,49 @@
     <t xml:space="preserve">1k</t>
   </si>
   <si>
+    <t xml:space="preserve">RC0402FR-071KL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-1.00KLRTR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">R33</t>
   </si>
   <si>
     <t xml:space="preserve">3R</t>
   </si>
   <si>
+    <t xml:space="preserve">RC0402FR-073RL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0402FR-073RL-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">R36</t>
   </si>
   <si>
     <t xml:space="preserve">56k</t>
   </si>
   <si>
+    <t xml:space="preserve">RC0402FR-0756KL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-56.0KLRTR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">S6</t>
   </si>
   <si>
-    <t xml:space="preserve">K1-5202UA-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Korean Hroparts</t>
+    <t xml:space="preserve">JS1400BFQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NINIGI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MICRO-JOY-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EG5858-ND </t>
   </si>
   <si>
     <t xml:space="preserve">C136710</t>
@@ -847,12 +904,21 @@
     <t xml:space="preserve">S3</t>
   </si>
   <si>
-    <t xml:space="preserve">K3-1296S-J1</t>
+    <t xml:space="preserve">CUS-12TB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nidec Copal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">563-1102-6-ND </t>
   </si>
   <si>
     <t xml:space="preserve">C223848</t>
   </si>
   <si>
+    <t xml:space="preserve">Slide switch, SPDT</t>
+  </si>
+  <si>
     <t xml:space="preserve">SW_SPDT_PCM12</t>
   </si>
   <si>
@@ -865,7 +931,10 @@
     <t xml:space="preserve">C&amp;K</t>
   </si>
   <si>
-    <t xml:space="preserve">PTS645SM43SMTR92 LFS</t>
+    <t xml:space="preserve"> PTS645SM50SMTR92 LFS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CKN10889TR-ND </t>
   </si>
   <si>
     <t xml:space="preserve">C393947</t>
@@ -1724,8 +1793,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C29" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3409,52 +3478,61 @@
       <c r="E32" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="F32" s="0" t="s">
+        <v>205</v>
+      </c>
       <c r="I32" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="K32" s="0" t="str">
+        <v>206</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K32" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B32*$O$79/J32,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L32" s="2" t="n">
         <f aca="false">IF(J32&gt;0,J32*K32,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
+      </c>
+      <c r="M32" s="3" t="n">
+        <v>0.12495</v>
       </c>
       <c r="N32" s="2" t="n">
         <f aca="false">L32*M32</f>
-        <v>0</v>
+        <v>71.2215</v>
       </c>
       <c r="O32" s="0" t="s">
         <v>113</v>
       </c>
       <c r="P32" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J33" s="2" t="n">
         <v>3000</v>
@@ -3492,25 +3570,25 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J34" s="2" t="n">
         <v>600</v>
@@ -3548,25 +3626,25 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J35" s="2" t="n">
         <v>600</v>
@@ -3604,25 +3682,25 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="J36" s="2" t="n">
         <v>600</v>
@@ -3657,22 +3735,22 @@
     </row>
     <row r="37" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B37" s="8" t="n">
         <v>6</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
       <c r="I37" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J37" s="11"/>
       <c r="K37" s="8" t="str">
@@ -3692,38 +3770,41 @@
         <v>113</v>
       </c>
       <c r="P37" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="Q37" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="S37" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AMI37" s="10"/>
       <c r="AMJ37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D38" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>236</v>
+      <c r="F38" s="0" t="s">
+        <v>239</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="J38" s="2" t="n">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="K38" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B38*$O$79/J38,0), "" )</f>
@@ -3731,23 +3812,23 @@
       </c>
       <c r="L38" s="2" t="n">
         <f aca="false">IF(J38&gt;0,J38*K38,$O$79)</f>
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="M38" s="3" t="n">
-        <v>0.05992</v>
+        <v>0.06067</v>
       </c>
       <c r="N38" s="2" t="n">
         <f aca="false">L38*M38</f>
-        <v>89.88</v>
+        <v>72.804</v>
       </c>
       <c r="O38" s="0" t="s">
         <v>113</v>
       </c>
       <c r="P38" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="S38" s="0" t="s">
         <v>130</v>
@@ -3755,22 +3836,25 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>246</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="J39" s="2" t="n">
         <v>3000</v>
@@ -3783,38 +3867,47 @@
         <f aca="false">IF(J39&gt;0,J39*K39,$O$79)</f>
         <v>3000</v>
       </c>
+      <c r="M39" s="3" t="n">
+        <v>0.01801</v>
+      </c>
       <c r="N39" s="2" t="n">
         <f aca="false">L39*M39</f>
-        <v>0</v>
+        <v>54.03</v>
+      </c>
+      <c r="O39" s="0" t="s">
+        <v>113</v>
       </c>
       <c r="P39" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>252</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="J40" s="2" t="n">
-        <v>3000</v>
+        <v>570</v>
       </c>
       <c r="K40" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B40*$O$79/J40,0), "" )</f>
@@ -3822,34 +3915,46 @@
       </c>
       <c r="L40" s="2" t="n">
         <f aca="false">IF(J40&gt;0,J40*K40,$O$79)</f>
-        <v>3000</v>
+        <v>570</v>
+      </c>
+      <c r="M40" s="3" t="n">
+        <v>0.1006</v>
       </c>
       <c r="N40" s="2" t="n">
         <f aca="false">L40*M40</f>
-        <v>0</v>
+        <v>57.342</v>
       </c>
       <c r="O40" s="0" t="s">
         <v>113</v>
       </c>
       <c r="P40" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>260</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="K41" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B41*$O$79/J41,0), "" )</f>
@@ -3857,31 +3962,43 @@
       </c>
       <c r="L41" s="0" t="n">
         <f aca="false">IF(J41&gt;0,J41*K41,$O$79)</f>
-        <v>15000</v>
+        <v>10000</v>
+      </c>
+      <c r="M41" s="3" t="n">
+        <v>0.00102</v>
       </c>
       <c r="N41" s="2" t="n">
         <f aca="false">L41*M41</f>
-        <v>0</v>
+        <v>10.2</v>
       </c>
       <c r="P41" s="0" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="Q41" s="0" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>257</v>
+        <v>264</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="K42" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B42*$O$79/J42,0), "" )</f>
@@ -3889,31 +4006,43 @@
       </c>
       <c r="L42" s="2" t="n">
         <f aca="false">IF(J42&gt;0,J42*K42,$O$79)</f>
-        <v>15000</v>
+        <v>10000</v>
+      </c>
+      <c r="M42" s="3" t="n">
+        <v>0.00188</v>
       </c>
       <c r="N42" s="2" t="n">
         <f aca="false">L42*M42</f>
-        <v>0</v>
+        <v>18.8</v>
       </c>
       <c r="P42" s="0" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>17</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>260</v>
+        <v>269</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>271</v>
       </c>
       <c r="J43" s="0" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="K43" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B43*$O$79/J43,0), "" )</f>
@@ -3921,31 +4050,43 @@
       </c>
       <c r="L43" s="2" t="n">
         <f aca="false">IF(J43&gt;0,J43*K43,$O$79)</f>
-        <v>15000</v>
+        <v>10000</v>
+      </c>
+      <c r="M43" s="3" t="n">
+        <v>0.00125</v>
       </c>
       <c r="N43" s="2" t="n">
         <f aca="false">L43*M43</f>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="P43" s="0" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>263</v>
+        <v>274</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>276</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="K44" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B44*$O$79/J44,0), "" )</f>
@@ -3953,31 +4094,43 @@
       </c>
       <c r="L44" s="2" t="n">
         <f aca="false">IF(J44&gt;0,J44*K44,$O$79)</f>
-        <v>15000</v>
+        <v>10000</v>
+      </c>
+      <c r="M44" s="3" t="n">
+        <v>0.00125</v>
       </c>
       <c r="N44" s="2" t="n">
         <f aca="false">L44*M44</f>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="P44" s="0" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>265</v>
+        <v>278</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>280</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="K45" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B45*$O$79/J45,0), "" )</f>
@@ -3985,31 +4138,43 @@
       </c>
       <c r="L45" s="2" t="n">
         <f aca="false">IF(J45&gt;0,J45*K45,$O$79)</f>
-        <v>15000</v>
+        <v>10000</v>
+      </c>
+      <c r="M45" s="3" t="n">
+        <v>0.00188</v>
       </c>
       <c r="N45" s="2" t="n">
         <f aca="false">L45*M45</f>
-        <v>0</v>
+        <v>18.8</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>267</v>
+        <v>282</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>284</v>
       </c>
       <c r="J46" s="0" t="n">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="K46" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B46*$O$79/J46,0), "" )</f>
@@ -4017,65 +4182,74 @@
       </c>
       <c r="L46" s="2" t="n">
         <f aca="false">IF(J46&gt;0,J46*K46,$O$79)</f>
-        <v>15000</v>
+        <v>10000</v>
+      </c>
+      <c r="M46" s="3" t="n">
+        <v>0.00125</v>
       </c>
       <c r="N46" s="2" t="n">
         <f aca="false">L46*M46</f>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="P46" s="26" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="B47" s="13" t="n">
         <v>1</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="F47" s="0"/>
+        <v>288</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>289</v>
+      </c>
       <c r="G47" s="0"/>
-      <c r="H47" s="0"/>
+      <c r="H47" s="13" t="s">
+        <v>288</v>
+      </c>
       <c r="I47" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="J47" s="2"/>
-      <c r="K47" s="0" t="str">
+        <v>290</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K47" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B47*$O$79/J47,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L47" s="2" t="n">
         <f aca="false">IF(J47&gt;0,J47*K47,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M47" s="3" t="n">
-        <v>0.277</v>
+        <v>0.68</v>
       </c>
       <c r="N47" s="2" t="n">
         <f aca="false">L47*M47</f>
-        <v>152.35</v>
+        <v>387.6</v>
       </c>
       <c r="O47" s="13" t="s">
         <v>30</v>
       </c>
       <c r="P47" s="13" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="Q47" s="14" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="AMD47" s="0"/>
       <c r="AME47" s="0"/>
@@ -4087,92 +4261,107 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>274</v>
+        <v>293</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>270</v>
+        <v>295</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>275</v>
+        <v>294</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>296</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="K48" s="0" t="str">
+        <v>297</v>
+      </c>
+      <c r="J48" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K48" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B48*$O$79/J48,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L48" s="2" t="n">
         <f aca="false">IF(J48&gt;0,J48*K48,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M48" s="3" t="n">
-        <v>0.05</v>
+        <v>0.36467</v>
       </c>
       <c r="N48" s="2" t="n">
         <f aca="false">L48*M48</f>
-        <v>27.5</v>
+        <v>207.8619</v>
       </c>
       <c r="O48" s="0" t="s">
         <v>113</v>
       </c>
+      <c r="P48" s="0" t="s">
+        <v>298</v>
+      </c>
       <c r="Q48" s="1" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
     </row>
     <row r="49" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="27" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="B49" s="27" t="n">
         <v>5</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>280</v>
+        <v>302</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>281</v>
-      </c>
-      <c r="F49" s="0"/>
+        <v>303</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>304</v>
+      </c>
       <c r="G49" s="0"/>
       <c r="H49" s="0"/>
       <c r="I49" s="27" t="s">
-        <v>282</v>
-      </c>
-      <c r="J49" s="29"/>
-      <c r="K49" s="27" t="str">
+        <v>305</v>
+      </c>
+      <c r="J49" s="29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="K49" s="27" t="n">
         <f aca="false">IFERROR( ROUNDUP(B49*$O$79/J49,0), "" )</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="L49" s="29" t="n">
         <f aca="false">IF(J49&gt;0,J49*K49,$O$79)</f>
-        <v>550</v>
-      </c>
-      <c r="M49" s="30"/>
+        <v>3000</v>
+      </c>
+      <c r="M49" s="30" t="n">
+        <v>0.10728</v>
+      </c>
       <c r="N49" s="2" t="n">
         <f aca="false">L49*M49</f>
-        <v>0</v>
+        <v>321.84</v>
       </c>
       <c r="O49" s="27" t="s">
         <v>113</v>
       </c>
       <c r="P49" s="27" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="Q49" s="27" t="s">
-        <v>284</v>
+        <v>307</v>
       </c>
       <c r="R49" s="27" t="s">
-        <v>285</v>
+        <v>308</v>
       </c>
       <c r="AMH49" s="0"/>
       <c r="AMI49" s="0"/>
@@ -4180,22 +4369,22 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>286</v>
+        <v>309</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="K50" s="0" t="str">
         <f aca="false">IFERROR( ROUNDUP(B50*$O$79/J50,0), "" )</f>
@@ -4216,27 +4405,27 @@
         <v>30</v>
       </c>
       <c r="P50" s="0" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>294</v>
+        <v>317</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>294</v>
+        <v>317</v>
       </c>
       <c r="I51" s="13"/>
       <c r="K51" s="0" t="str">
@@ -4258,28 +4447,28 @@
         <v>198</v>
       </c>
       <c r="P51" s="0" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>297</v>
+        <v>320</v>
       </c>
       <c r="R51" s="13"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>298</v>
+        <v>321</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="I52" s="13"/>
       <c r="K52" s="0" t="str">
@@ -4301,27 +4490,27 @@
         <v>30</v>
       </c>
       <c r="P52" s="0" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
     </row>
     <row r="53" s="34" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="31" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="B53" s="31" t="n">
         <v>1</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="E53" s="32" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="F53" s="0"/>
       <c r="G53" s="0"/>
@@ -4347,10 +4536,10 @@
         <v>30</v>
       </c>
       <c r="P53" s="31" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="Q53" s="32" t="s">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="R53" s="31"/>
       <c r="T53" s="31"/>
@@ -4360,19 +4549,19 @@
     </row>
     <row r="54" s="31" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="31" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="B54" s="31" t="n">
         <v>1</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="F54" s="0"/>
       <c r="G54" s="0"/>
@@ -4397,7 +4586,7 @@
         <v>198</v>
       </c>
       <c r="P54" s="31" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="Q54" s="32"/>
       <c r="AMD54" s="34"/>
@@ -4410,19 +4599,19 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>314</v>
+        <v>337</v>
       </c>
       <c r="J55" s="0"/>
       <c r="K55" s="0" t="str">
@@ -4445,30 +4634,30 @@
         <v>198</v>
       </c>
       <c r="P55" s="0" t="s">
-        <v>315</v>
+        <v>338</v>
       </c>
       <c r="Q55" s="0" t="s">
-        <v>316</v>
+        <v>339</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>317</v>
+        <v>340</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>318</v>
+        <v>341</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>319</v>
+        <v>342</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>320</v>
+        <v>343</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>321</v>
+        <v>344</v>
       </c>
       <c r="K56" s="0" t="str">
         <f aca="false">IFERROR( ROUNDUP(B56*$O$79/J56,0), "" )</f>
@@ -4489,28 +4678,28 @@
         <v>113</v>
       </c>
       <c r="P56" s="0" t="s">
-        <v>322</v>
+        <v>345</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>323</v>
+        <v>346</v>
       </c>
       <c r="R56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>324</v>
+        <v>347</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>325</v>
+        <v>348</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
       <c r="K57" s="0" t="str">
         <f aca="false">IFERROR( ROUNDUP(B57*$O$79/J57,0), "" )</f>
@@ -4531,30 +4720,30 @@
         <v>30</v>
       </c>
       <c r="P57" s="0" t="s">
-        <v>327</v>
+        <v>350</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>328</v>
+        <v>351</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>332</v>
+        <v>355</v>
       </c>
       <c r="K58" s="0" t="str">
         <f aca="false">IFERROR( ROUNDUP(B58*$O$79/J58,0), "" )</f>
@@ -4575,30 +4764,30 @@
         <v>30</v>
       </c>
       <c r="P58" s="0" t="s">
-        <v>333</v>
+        <v>356</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>334</v>
+        <v>357</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>335</v>
+        <v>358</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>336</v>
+        <v>359</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>337</v>
+        <v>360</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>338</v>
+        <v>361</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>339</v>
+        <v>362</v>
       </c>
       <c r="K59" s="0" t="str">
         <f aca="false">IFERROR( ROUNDUP(B59*$O$79/J59,0), "" )</f>
@@ -4619,30 +4808,30 @@
         <v>30</v>
       </c>
       <c r="P59" s="0" t="s">
-        <v>340</v>
+        <v>363</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>341</v>
+        <v>364</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>343</v>
+        <v>366</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>337</v>
+        <v>360</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>344</v>
+        <v>367</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>345</v>
+        <v>368</v>
       </c>
       <c r="K60" s="0" t="str">
         <f aca="false">IFERROR( ROUNDUP(B60*$O$79/J60,0), "" )</f>
@@ -4663,10 +4852,10 @@
         <v>30</v>
       </c>
       <c r="P60" s="0" t="s">
-        <v>346</v>
+        <v>369</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>347</v>
+        <v>370</v>
       </c>
       <c r="R60" s="0" t="s">
         <v>44</v>
@@ -4690,19 +4879,19 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>348</v>
+        <v>371</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>349</v>
+        <v>372</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>350</v>
+        <v>373</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>351</v>
+        <v>374</v>
       </c>
       <c r="J62" s="0"/>
       <c r="K62" s="0" t="str">
@@ -4724,25 +4913,25 @@
         <v>30</v>
       </c>
       <c r="P62" s="0" t="s">
-        <v>352</v>
+        <v>375</v>
       </c>
       <c r="Q62" s="0"/>
     </row>
     <row r="63" s="31" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="31" t="s">
-        <v>353</v>
+        <v>376</v>
       </c>
       <c r="B63" s="31" t="n">
         <v>1</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>349</v>
+        <v>372</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>354</v>
+        <v>377</v>
       </c>
       <c r="E63" s="32" t="s">
-        <v>355</v>
+        <v>378</v>
       </c>
       <c r="F63" s="0"/>
       <c r="G63" s="0"/>
@@ -4767,7 +4956,7 @@
         <v>30</v>
       </c>
       <c r="P63" s="31" t="s">
-        <v>356</v>
+        <v>379</v>
       </c>
       <c r="AMD63" s="34"/>
       <c r="AME63" s="34"/>
@@ -4779,13 +4968,13 @@
     </row>
     <row r="64" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="27" t="s">
-        <v>357</v>
+        <v>380</v>
       </c>
       <c r="B64" s="27" t="n">
         <v>1</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>349</v>
+        <v>372</v>
       </c>
       <c r="E64" s="28"/>
       <c r="F64" s="0"/>
@@ -4813,16 +5002,16 @@
     </row>
     <row r="65" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="27" t="s">
-        <v>358</v>
+        <v>381</v>
       </c>
       <c r="B65" s="27" t="n">
         <v>1</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>349</v>
+        <v>372</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="E65" s="28"/>
       <c r="F65" s="0"/>
@@ -4845,10 +5034,10 @@
         <v>330</v>
       </c>
       <c r="P65" s="27" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="R65" s="27" t="s">
-        <v>285</v>
+        <v>308</v>
       </c>
       <c r="AMH65" s="0"/>
       <c r="AMI65" s="0"/>
@@ -4856,7 +5045,7 @@
     </row>
     <row r="66" s="31" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="31" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="B66" s="31" t="n">
         <v>1</v>
@@ -4891,17 +5080,17 @@
     </row>
     <row r="67" s="31" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="31" t="s">
-        <v>362</v>
+        <v>385</v>
       </c>
       <c r="B67" s="31" t="n">
         <v>1</v>
       </c>
       <c r="C67" s="32"/>
       <c r="D67" s="31" t="s">
-        <v>363</v>
+        <v>386</v>
       </c>
       <c r="E67" s="32" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
       <c r="F67" s="0"/>
       <c r="G67" s="0"/>
@@ -4933,7 +5122,7 @@
     </row>
     <row r="68" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="17" t="s">
-        <v>365</v>
+        <v>388</v>
       </c>
       <c r="B68" s="17" t="n">
         <v>1</v>
@@ -4970,7 +5159,7 @@
     </row>
     <row r="69" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="17" t="s">
-        <v>366</v>
+        <v>389</v>
       </c>
       <c r="B69" s="17" t="n">
         <v>1</v>
@@ -5013,7 +5202,7 @@
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
       <c r="M72" s="7" t="s">
-        <v>367</v>
+        <v>390</v>
       </c>
       <c r="N72" s="6" t="e">
         <f aca="false">SUM(N2:N71)</f>
@@ -5023,7 +5212,7 @@
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L73" s="6"/>
       <c r="M73" s="7" t="s">
-        <v>368</v>
+        <v>391</v>
       </c>
       <c r="N73" s="6" t="e">
         <f aca="false">N72/$O$79</f>
@@ -5032,7 +5221,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>369</v>
+        <v>392</v>
       </c>
       <c r="B74" s="0" t="n">
         <f aca="false">SUM(B2:B73)</f>
@@ -5044,18 +5233,18 @@
         <v>113</v>
       </c>
       <c r="P75" s="0" t="s">
-        <v>370</v>
+        <v>393</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L76" s="6" t="s">
-        <v>371</v>
+        <v>394</v>
       </c>
       <c r="O76" s="0" t="s">
         <v>30</v>
       </c>
       <c r="P76" s="0" t="s">
-        <v>372</v>
+        <v>395</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5063,7 +5252,7 @@
         <v>198</v>
       </c>
       <c r="P77" s="0" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5071,24 +5260,24 @@
         <v>550</v>
       </c>
       <c r="P79" s="0" t="s">
-        <v>374</v>
+        <v>397</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="37" t="s">
-        <v>375</v>
+        <v>398</v>
       </c>
       <c r="C80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="38" t="s">
-        <v>376</v>
+        <v>399</v>
       </c>
       <c r="C81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="39" t="s">
-        <v>377</v>
+        <v>400</v>
       </c>
       <c r="C82" s="0"/>
     </row>

</xml_diff>

<commit_message>
All parts researched, most parts sourced, total price estimate probably a decent estimate
</commit_message>
<xml_diff>
--- a/r2/bom/tr20-r2-alternative-sources.xlsx
+++ b/r2/bom/tr20-r2-alternative-sources.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="426">
   <si>
     <t xml:space="preserve">References</t>
   </si>
@@ -109,6 +109,9 @@
     <t xml:space="preserve">GRM1557U1A152JA01D</t>
   </si>
   <si>
+    <t xml:space="preserve">490-10690-6-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">C162143</t>
   </si>
   <si>
@@ -121,7 +124,7 @@
     <t xml:space="preserve">C_0402_1005Metric</t>
   </si>
   <si>
-    <t xml:space="preserve">Critical – U2J, UJ, C0G only. (X7R is not suitable)</t>
+    <t xml:space="preserve">Critical – U2J, UJ, C0G only</t>
   </si>
   <si>
     <t xml:space="preserve">C3 C5 C11 C25 C26 C27 C28 C29 C30 C31 C34 C38 C41 C42 C75</t>
@@ -460,6 +463,9 @@
     <t xml:space="preserve">IDC-Header_2x05_P2.54mm_Vertical_SMD</t>
   </si>
   <si>
+    <t xml:space="preserve">DNP – not required</t>
+  </si>
+  <si>
     <t xml:space="preserve">J1 J9</t>
   </si>
   <si>
@@ -718,6 +724,9 @@
     <t xml:space="preserve">SK6812/WS2812B-Mini </t>
   </si>
   <si>
+    <t xml:space="preserve">WS2812B-MINI</t>
+  </si>
+  <si>
     <t xml:space="preserve">C114583</t>
   </si>
   <si>
@@ -727,7 +736,7 @@
     <t xml:space="preserve">LED_SK6812MINI_PLCC4_3.5x3.5mm_P1.75mm_no_silk</t>
   </si>
   <si>
-    <t xml:space="preserve">Hard to find…</t>
+    <t xml:space="preserve">Hard to fiind, no stock at TME, only hobby products at Digikey, Mouser (Adafruit, Sparkfun, etc)</t>
   </si>
   <si>
     <t xml:space="preserve">Q4 Q5</t>
@@ -901,6 +910,9 @@
     <t xml:space="preserve">SW_JS1400BFQ-arrows</t>
   </si>
   <si>
+    <t xml:space="preserve">Unknown packaging</t>
+  </si>
+  <si>
     <t xml:space="preserve">S3</t>
   </si>
   <si>
@@ -931,7 +943,7 @@
     <t xml:space="preserve">C&amp;K</t>
   </si>
   <si>
-    <t xml:space="preserve"> PTS645SM50SMTR92 LFS </t>
+    <t xml:space="preserve">PTS645SM50SMTR92 LFS </t>
   </si>
   <si>
     <t xml:space="preserve">CKN10889TR-ND </t>
@@ -946,9 +958,6 @@
     <t xml:space="preserve">Switch_Tactile_SMD_6x6mm_PTS645</t>
   </si>
   <si>
-    <t xml:space="preserve">Yellow possible? Pantone 1375C</t>
-  </si>
-  <si>
     <t xml:space="preserve">U2</t>
   </si>
   <si>
@@ -961,6 +970,9 @@
     <t xml:space="preserve">AP2114H-3.3TRG1</t>
   </si>
   <si>
+    <t xml:space="preserve">AP2114H-3.3TRG1DIDKR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">C150716</t>
   </si>
   <si>
@@ -979,6 +991,12 @@
     <t xml:space="preserve">Texas Instruments</t>
   </si>
   <si>
+    <t xml:space="preserve">CC1200RHBR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-38892-6-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">Low-Power, High-Performance RF Transceiver, QFN-32</t>
   </si>
   <si>
@@ -988,12 +1006,15 @@
     <t xml:space="preserve">U3</t>
   </si>
   <si>
-    <t xml:space="preserve">CP2102N-A01-GQFN24</t>
+    <t xml:space="preserve">CP2102N-A02-GQFN24R </t>
   </si>
   <si>
     <t xml:space="preserve">Si Labs</t>
   </si>
   <si>
+    <t xml:space="preserve">336-5888-6-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">USB to UART master bridge, QFN-24</t>
   </si>
   <si>
@@ -1006,6 +1027,12 @@
     <t xml:space="preserve">DRV2605LDGS</t>
   </si>
   <si>
+    <t xml:space="preserve">DRV2605LDGSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-40032-6-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">I2C haptic driver</t>
   </si>
   <si>
@@ -1024,6 +1051,9 @@
     <t xml:space="preserve">2.9” e-paper display</t>
   </si>
   <si>
+    <t xml:space="preserve">Unlikely that these exist outside China</t>
+  </si>
+  <si>
     <t xml:space="preserve">U6</t>
   </si>
   <si>
@@ -1054,6 +1084,9 @@
     <t xml:space="preserve">MCP73831T-3ACI/OT</t>
   </si>
   <si>
+    <t xml:space="preserve">MCP73831T-3ACI/OTDKR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">C14879</t>
   </si>
   <si>
@@ -1072,6 +1105,9 @@
     <t xml:space="preserve">PCA9555PW,112</t>
   </si>
   <si>
+    <t xml:space="preserve">568-3986-5-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">I2C IO Expander, with internal pull-ups</t>
   </si>
   <si>
@@ -1087,6 +1123,9 @@
     <t xml:space="preserve">PCM5100APWR</t>
   </si>
   <si>
+    <t xml:space="preserve">296-36705-6-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">C131154</t>
   </si>
   <si>
@@ -1108,6 +1147,9 @@
     <t xml:space="preserve">Q13FC1350000200</t>
   </si>
   <si>
+    <t xml:space="preserve">SER4103DKR-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">C48615</t>
   </si>
   <si>
@@ -1123,7 +1165,10 @@
     <t xml:space="preserve">40Mhz</t>
   </si>
   <si>
-    <t xml:space="preserve">X1E000021017700</t>
+    <t xml:space="preserve">NX3225SA 40MHz EXS00A-CS03880 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">644-1249-1-ND </t>
   </si>
   <si>
     <t xml:space="preserve">C255943</t>
@@ -1138,18 +1183,18 @@
     <t xml:space="preserve">Linear Resonant Actuator</t>
   </si>
   <si>
-    <t xml:space="preserve">DNP, user supplied</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ineed Youngsun Technology Co., Ltd. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0832BE03L15</t>
+    <t xml:space="preserve">Precision Microdrives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C08-00A</t>
   </si>
   <si>
     <t xml:space="preserve">Linear Resonant Actuator Ø8x3.2T, 235Hz, 1.8Vrms AC</t>
   </si>
   <si>
+    <t xml:space="preserve">UK manufacturer. Expensive, not enough stock, but might be able to produce more</t>
+  </si>
+  <si>
     <t xml:space="preserve">Batt</t>
   </si>
   <si>
@@ -1162,34 +1207,55 @@
     <t xml:space="preserve">1500mAh Lipo with Molex 510210200, 50mm wire length</t>
   </si>
   <si>
+    <t xml:space="preserve">OMG I hate UPS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Earbuds</t>
   </si>
   <si>
+    <t xml:space="preserve">Double check with Kerstin</t>
+  </si>
+  <si>
     <t xml:space="preserve">USB-C cable</t>
   </si>
   <si>
-    <t xml:space="preserve">San Guan Siyuan</t>
+    <t xml:space="preserve">San Guan Siyuan?</t>
   </si>
   <si>
     <t xml:space="preserve">Custom, 0.75m</t>
   </si>
   <si>
+    <t xml:space="preserve">Waiting to hear from Sally, Abby (CN)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inkjet printing</t>
   </si>
   <si>
+    <t xml:space="preserve">Peerless Coatings?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFQ out to Peerless Coatings Ltd.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Laser cut coverlay</t>
   </si>
   <si>
-    <t xml:space="preserve">SZ Chong Ming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tr20-coverlay</t>
+    <t xml:space="preserve">PCB Fabrication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown vendor, EU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In progress</t>
   </si>
   <si>
     <t xml:space="preserve">PCB Assembly</t>
   </si>
   <si>
-    <t xml:space="preserve">PCB Fabrication</t>
+    <t xml:space="preserve">HCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need components from around 22/2</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -1213,16 +1279,25 @@
     <t xml:space="preserve">Do not substitute</t>
   </si>
   <si>
+    <t xml:space="preserve">TODO: compare against tr20-r2.xlsx – missing the 5.1k resistors. Is something else missing ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Units to build</t>
   </si>
   <si>
-    <t xml:space="preserve">Attention Allnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attention Jeff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Custom colour specification</t>
+    <t xml:space="preserve">Question / Noite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical / Problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore – Part not required</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1431,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1384,7 +1459,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFF7D1D5"/>
       </patternFill>
     </fill>
     <fill>
@@ -1396,19 +1471,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFA6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFB66C"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <fgColor rgb="FFFFFFA6"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -1425,14 +1500,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE8A202"/>
-        <bgColor rgb="FFFFCC00"/>
+        <fgColor rgb="FFFFB66C"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD7D7"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFF7D1D5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7D1D5"/>
+        <bgColor rgb="FFFFD7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4000"/>
+        <bgColor rgb="FFCC0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1536,7 +1623,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1641,23 +1728,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1669,6 +1784,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1681,7 +1800,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1689,11 +1844,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1744,7 +1907,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -1758,9 +1921,9 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFF7D1D5"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFD7D7"/>
+      <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFFB66C"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -1769,8 +1932,8 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFE8A202"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -1793,8 +1956,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C29" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F45" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I72" activeCellId="0" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1803,7 +1966,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.64"/>
@@ -1816,8 +1979,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="47.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="52.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="41.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="73.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="24.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="34.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="41.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
@@ -1933,7 +2096,7 @@
         <v>24</v>
       </c>
       <c r="AMI2" s="10"/>
-      <c r="AMJ2" s="0"/>
+      <c r="AMJ2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -1951,11 +2114,14 @@
       <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="I3" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>10000</v>
+        <v>600</v>
       </c>
       <c r="K3" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B3*$O$79/J3,0), "" )</f>
@@ -1963,43 +2129,46 @@
       </c>
       <c r="L3" s="2" t="n">
         <f aca="false">IF(J3&gt;0,J3*K3,$O$79)</f>
-        <v>10000</v>
+        <v>600</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>0.15</v>
       </c>
       <c r="N3" s="2" t="n">
         <f aca="false">L3*M3</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="13" t="n">
         <v>15</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
@@ -2022,7 +2191,7 @@
         <v>33.5</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AMD4" s="0"/>
       <c r="AME4" s="0"/>
@@ -2034,22 +2203,22 @@
     </row>
     <row r="5" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="13" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G5" s="0"/>
       <c r="H5" s="0"/>
@@ -2072,13 +2241,13 @@
         <v>44.8</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R5" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AMD5" s="0"/>
       <c r="AME5" s="0"/>
@@ -2090,22 +2259,22 @@
     </row>
     <row r="6" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G6" s="0"/>
       <c r="H6" s="0"/>
@@ -2128,10 +2297,10 @@
         <v>27.4</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AMD6" s="0"/>
       <c r="AME6" s="0"/>
@@ -2143,22 +2312,22 @@
     </row>
     <row r="7" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" s="13" t="n">
         <v>5</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
@@ -2181,13 +2350,13 @@
         <v>44.9</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AMD7" s="0"/>
       <c r="AME7" s="0"/>
@@ -2199,22 +2368,22 @@
     </row>
     <row r="8" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
@@ -2237,13 +2406,13 @@
         <v>70.6</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R8" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AMD8" s="0"/>
       <c r="AME8" s="0"/>
@@ -2255,22 +2424,22 @@
     </row>
     <row r="9" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" s="13" t="n">
         <v>23</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
@@ -2293,13 +2462,13 @@
         <v>263.68</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AMD9" s="0"/>
       <c r="AME9" s="0"/>
@@ -2311,22 +2480,22 @@
     </row>
     <row r="10" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" s="13" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
@@ -2349,13 +2518,13 @@
         <v>44.8</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R10" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AMD10" s="0"/>
       <c r="AME10" s="0"/>
@@ -2367,22 +2536,22 @@
     </row>
     <row r="11" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="13" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
@@ -2405,10 +2574,10 @@
         <v>87.4</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AMD11" s="0"/>
       <c r="AME11" s="0"/>
@@ -2420,22 +2589,22 @@
     </row>
     <row r="12" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B12" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
@@ -2458,10 +2627,10 @@
         <v>406.02</v>
       </c>
       <c r="P12" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AMD12" s="0"/>
       <c r="AME12" s="0"/>
@@ -2473,22 +2642,22 @@
     </row>
     <row r="13" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B13" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
@@ -2511,13 +2680,13 @@
         <v>122.2</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q13" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AMD13" s="0"/>
       <c r="AME13" s="0"/>
@@ -2529,22 +2698,22 @@
     </row>
     <row r="14" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B14" s="13" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
@@ -2567,13 +2736,13 @@
         <v>44.6</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R14" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AMD14" s="0"/>
       <c r="AME14" s="0"/>
@@ -2585,22 +2754,22 @@
     </row>
     <row r="15" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B15" s="13" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
@@ -2623,13 +2792,13 @@
         <v>70.6</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q15" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R15" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AMD15" s="0"/>
       <c r="AME15" s="0"/>
@@ -2641,22 +2810,22 @@
     </row>
     <row r="16" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B16" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
@@ -2679,13 +2848,13 @@
         <v>149.56</v>
       </c>
       <c r="P16" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q16" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R16" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AMD16" s="0"/>
       <c r="AME16" s="0"/>
@@ -2697,22 +2866,22 @@
     </row>
     <row r="17" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B17" s="13" t="n">
         <v>11</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
@@ -2735,13 +2904,13 @@
         <v>80.2</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q17" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AMD17" s="0"/>
       <c r="AME17" s="0"/>
@@ -2753,25 +2922,25 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F18" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J18" s="2" t="n">
         <v>8000</v>
@@ -2792,36 +2961,36 @@
         <v>201.68</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B19" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J19" s="19" t="n">
         <v>600</v>
@@ -2842,40 +3011,39 @@
         <v>43.338</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P19" s="17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q19" s="18" t="n">
         <v>1206</v>
       </c>
       <c r="S19" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="AMJ19" s="0"/>
+        <v>124</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J20" s="2" t="n">
         <v>3000</v>
@@ -2895,39 +3063,39 @@
         <v>43.338</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q20" s="1" t="n">
         <v>1206</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="F21" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J21" s="2" t="n">
         <v>3000</v>
@@ -2948,36 +3116,36 @@
         <v>143.37</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J22" s="2" t="n">
         <v>3000</v>
@@ -2997,33 +3165,33 @@
         <v>43.338</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Q22" s="1" t="n">
         <v>1206</v>
       </c>
       <c r="S22" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B23" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D23" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>144</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>143</v>
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
@@ -3042,17 +3210,20 @@
         <v>0</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Q23" s="21" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="S23" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="AMI23" s="23"/>
-      <c r="AMJ23" s="0"/>
+      <c r="AMJ23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>2</v>
@@ -3061,16 +3232,16 @@
         <v>532610271</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E24" s="1" t="n">
         <v>532610271</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>1200</v>
@@ -3091,36 +3262,36 @@
         <v>223.2</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="S24" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B25" s="13" t="n">
         <v>1</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="J25" s="2" t="n">
         <v>600</v>
@@ -3141,38 +3312,38 @@
         <v>294</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B26" s="13" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="0"/>
       <c r="I26" s="13" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J26" s="16" t="n">
         <v>570</v>
@@ -3193,10 +3364,10 @@
         <v>864.519</v>
       </c>
       <c r="O26" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Q26" s="14" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AMD26" s="0"/>
       <c r="AME26" s="0"/>
@@ -3208,25 +3379,25 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J27" s="2" t="n">
         <v>570</v>
@@ -3247,36 +3418,36 @@
         <v>315.5064</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="J28" s="2" t="n">
         <v>1000</v>
@@ -3297,36 +3468,36 @@
         <v>570</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E29" s="1" t="n">
         <v>629104190121</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>570</v>
@@ -3347,36 +3518,36 @@
         <v>442.4283</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="Q29" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J30" s="2" t="n">
         <v>570</v>
@@ -3397,36 +3568,36 @@
         <v>432.63</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="J31" s="2" t="n">
         <v>600</v>
@@ -3447,42 +3618,42 @@
         <v>44.04</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="P31" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="R31" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S31" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="J32" s="2" t="n">
         <v>570</v>
@@ -3503,36 +3674,36 @@
         <v>71.2215</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P32" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="J33" s="2" t="n">
         <v>3000</v>
@@ -3553,42 +3724,42 @@
         <v>146.82</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="P33" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="R33" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S33" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="J34" s="2" t="n">
         <v>600</v>
@@ -3609,42 +3780,42 @@
         <v>44.04</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="P34" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="R34" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S34" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="J35" s="2" t="n">
         <v>600</v>
@@ -3665,42 +3836,42 @@
         <v>44.04</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="P35" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="R35" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S35" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="J36" s="2" t="n">
         <v>600</v>
@@ -3721,87 +3892,93 @@
         <v>47.988</v>
       </c>
       <c r="O36" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="P36" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="R36" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="B37" s="8" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B37" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="8" t="s">
+      <c r="C37" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="J37" s="11"/>
-      <c r="K37" s="8" t="str">
+      <c r="E37" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="I37" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="J37" s="29" t="n">
+        <v>900</v>
+      </c>
+      <c r="K37" s="26" t="n">
         <f aca="false">IFERROR( ROUNDUP(B37*$O$79/J37,0), "" )</f>
-        <v/>
-      </c>
-      <c r="L37" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="L37" s="29" t="n">
         <f aca="false">IF(J37&gt;0,J37*K37,$O$79)</f>
-        <v>550</v>
-      </c>
-      <c r="M37" s="12"/>
-      <c r="N37" s="11" t="n">
+        <v>3600</v>
+      </c>
+      <c r="M37" s="30" t="n">
+        <v>0.0983</v>
+      </c>
+      <c r="N37" s="29" t="n">
         <f aca="false">L37*M37</f>
-        <v>0</v>
-      </c>
-      <c r="O37" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="P37" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q37" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="S37" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="AMI37" s="10"/>
+        <v>353.88</v>
+      </c>
+      <c r="O37" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="P37" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q37" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="S37" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="AMI37" s="28"/>
       <c r="AMJ37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="J38" s="2" t="n">
         <v>1200</v>
@@ -3822,39 +3999,39 @@
         <v>72.804</v>
       </c>
       <c r="O38" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P38" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="S38" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="J39" s="2" t="n">
         <v>3000</v>
@@ -3875,36 +4052,36 @@
         <v>54.03</v>
       </c>
       <c r="O39" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P39" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="J40" s="2" t="n">
         <v>570</v>
@@ -3925,33 +4102,33 @@
         <v>57.342</v>
       </c>
       <c r="O40" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P40" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="J41" s="0" t="n">
         <v>10000</v>
@@ -3972,30 +4149,30 @@
         <v>10.2</v>
       </c>
       <c r="P41" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="Q41" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>10000</v>
@@ -4016,30 +4193,30 @@
         <v>18.8</v>
       </c>
       <c r="P42" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>17</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>10000</v>
@@ -4060,30 +4237,30 @@
         <v>12.5</v>
       </c>
       <c r="P43" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>10000</v>
@@ -4104,30 +4281,30 @@
         <v>12.5</v>
       </c>
       <c r="P44" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="J45" s="0" t="n">
         <v>10000</v>
@@ -4148,30 +4325,30 @@
         <v>18.8</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="J46" s="0" t="n">
         <v>10000</v>
@@ -4191,38 +4368,38 @@
         <f aca="false">L46*M46</f>
         <v>12.5</v>
       </c>
-      <c r="P46" s="26" t="s">
-        <v>261</v>
+      <c r="P46" s="31" t="s">
+        <v>264</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="47" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B47" s="13" t="n">
         <v>1</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G47" s="0"/>
       <c r="H47" s="13" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="J47" s="2" t="n">
         <v>570</v>
@@ -4243,13 +4420,16 @@
         <v>387.6</v>
       </c>
       <c r="O47" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P47" s="13" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="Q47" s="14" t="s">
-        <v>292</v>
+        <v>295</v>
+      </c>
+      <c r="S47" s="13" t="s">
+        <v>296</v>
       </c>
       <c r="AMD47" s="0"/>
       <c r="AME47" s="0"/>
@@ -4261,25 +4441,25 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="J48" s="2" t="n">
         <v>570</v>
@@ -4300,570 +4480,645 @@
         <v>207.8619</v>
       </c>
       <c r="O48" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P48" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="49" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="B49" s="27" t="n">
+        <v>303</v>
+      </c>
+      <c r="S48" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B49" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C49" s="27" t="s">
-        <v>301</v>
-      </c>
-      <c r="D49" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>303</v>
+      <c r="C49" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>307</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="G49" s="0"/>
-      <c r="H49" s="0"/>
-      <c r="I49" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="J49" s="29" t="n">
+        <v>308</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="J49" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="K49" s="27" t="n">
+      <c r="K49" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B49*$O$79/J49,0), "" )</f>
         <v>3</v>
       </c>
-      <c r="L49" s="29" t="n">
+      <c r="L49" s="0" t="n">
         <f aca="false">IF(J49&gt;0,J49*K49,$O$79)</f>
         <v>3000</v>
       </c>
-      <c r="M49" s="30" t="n">
+      <c r="M49" s="0" t="n">
         <v>0.10728</v>
       </c>
-      <c r="N49" s="2" t="n">
+      <c r="N49" s="0" t="n">
         <f aca="false">L49*M49</f>
         <v>321.84</v>
       </c>
-      <c r="O49" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="P49" s="27" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q49" s="27" t="s">
-        <v>307</v>
-      </c>
-      <c r="R49" s="27" t="s">
-        <v>308</v>
-      </c>
-      <c r="AMH49" s="0"/>
-      <c r="AMI49" s="0"/>
-      <c r="AMJ49" s="0"/>
+      <c r="O49" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="P49" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q49" s="0" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>312</v>
+        <v>315</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>316</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="K50" s="0" t="str">
+        <v>317</v>
+      </c>
+      <c r="J50" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K50" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B50*$O$79/J50,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L50" s="2" t="n">
         <f aca="false">IF(J50&gt;0,J50*K50,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M50" s="3" t="n">
-        <v>0.06</v>
+        <v>0.11363</v>
       </c>
       <c r="N50" s="2" t="n">
         <f aca="false">L50*M50</f>
-        <v>33</v>
+        <v>64.7691</v>
       </c>
       <c r="O50" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P50" s="0" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>315</v>
+        <v>319</v>
+      </c>
+      <c r="S50" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>317</v>
+        <v>323</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>324</v>
       </c>
       <c r="I51" s="13"/>
-      <c r="K51" s="0" t="str">
+      <c r="J51" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K51" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B51*$O$79/J51,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L51" s="2" t="n">
         <f aca="false">IF(J51&gt;0,J51*K51,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M51" s="3" t="n">
-        <v>3.22</v>
+        <v>2.46846</v>
       </c>
       <c r="N51" s="2" t="n">
         <f aca="false">L51*M51</f>
-        <v>1771</v>
+        <v>1407.0222</v>
       </c>
       <c r="O51" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="P51" s="0" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="R51" s="13"/>
+      <c r="S51" s="0" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>322</v>
+        <v>328</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>330</v>
       </c>
       <c r="I52" s="13"/>
-      <c r="K52" s="0" t="str">
+      <c r="J52" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K52" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B52*$O$79/J52,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L52" s="2" t="n">
         <f aca="false">IF(J52&gt;0,J52*K52,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M52" s="3" t="n">
-        <v>1.25</v>
+        <v>0.96609</v>
       </c>
       <c r="N52" s="2" t="n">
         <f aca="false">L52*M52</f>
-        <v>687.5</v>
+        <v>550.6713</v>
       </c>
       <c r="O52" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P52" s="0" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="53" s="34" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="31" t="s">
-        <v>326</v>
-      </c>
-      <c r="B53" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" s="32" t="s">
-        <v>327</v>
-      </c>
-      <c r="D53" s="31" t="s">
-        <v>318</v>
-      </c>
-      <c r="E53" s="32" t="s">
-        <v>327</v>
-      </c>
-      <c r="F53" s="0"/>
-      <c r="G53" s="0"/>
-      <c r="H53" s="0"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="33"/>
-      <c r="K53" s="34" t="str">
+        <v>332</v>
+      </c>
+      <c r="S52" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="B53" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="E53" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="34" t="n">
+        <v>570</v>
+      </c>
+      <c r="K53" s="35" t="n">
         <f aca="false">IFERROR( ROUNDUP(B53*$O$79/J53,0), "" )</f>
-        <v/>
-      </c>
-      <c r="L53" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="L53" s="34" t="n">
         <f aca="false">IF(J53&gt;0,J53*K53,$O$79)</f>
-        <v>550</v>
-      </c>
-      <c r="M53" s="35" t="n">
-        <v>1.65</v>
-      </c>
-      <c r="N53" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="M53" s="36" t="n">
+        <v>1.27058</v>
+      </c>
+      <c r="N53" s="34" t="n">
         <f aca="false">L53*M53</f>
-        <v>907.5</v>
-      </c>
-      <c r="O53" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="P53" s="31" t="s">
-        <v>328</v>
-      </c>
-      <c r="Q53" s="32" t="s">
-        <v>329</v>
-      </c>
-      <c r="R53" s="31"/>
-      <c r="T53" s="31"/>
-      <c r="AMH53" s="0"/>
-      <c r="AMI53" s="0"/>
-      <c r="AMJ53" s="0"/>
-    </row>
-    <row r="54" s="31" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="31" t="s">
-        <v>330</v>
-      </c>
-      <c r="B54" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C54" s="31" t="s">
-        <v>331</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>332</v>
-      </c>
-      <c r="E54" s="32" t="s">
-        <v>331</v>
-      </c>
-      <c r="F54" s="0"/>
-      <c r="G54" s="0"/>
-      <c r="H54" s="0"/>
-      <c r="J54" s="33"/>
-      <c r="K54" s="34" t="str">
+        <v>724.2306</v>
+      </c>
+      <c r="O53" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="P53" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q53" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="R53" s="32"/>
+      <c r="S53" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="T53" s="32"/>
+      <c r="AMH53" s="37"/>
+      <c r="AMI53" s="32"/>
+      <c r="AMJ53" s="32"/>
+    </row>
+    <row r="54" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="B54" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="D54" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="E54" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="42" t="str">
         <f aca="false">IFERROR( ROUNDUP(B54*$O$79/J54,0), "" )</f>
         <v/>
       </c>
-      <c r="L54" s="33" t="n">
+      <c r="L54" s="41" t="n">
         <f aca="false">IF(J54&gt;0,J54*K54,$O$79)</f>
         <v>550</v>
       </c>
-      <c r="M54" s="35" t="n">
+      <c r="M54" s="43" t="n">
         <v>6</v>
       </c>
-      <c r="N54" s="2" t="n">
+      <c r="N54" s="41" t="n">
         <f aca="false">L54*M54</f>
         <v>3300</v>
       </c>
-      <c r="O54" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="P54" s="31" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q54" s="32"/>
-      <c r="AMD54" s="34"/>
-      <c r="AME54" s="34"/>
-      <c r="AMF54" s="34"/>
-      <c r="AMG54" s="34"/>
-      <c r="AMH54" s="0"/>
-      <c r="AMI54" s="0"/>
-      <c r="AMJ54" s="0"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="B55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="J55" s="0"/>
-      <c r="K55" s="0" t="str">
+      <c r="O54" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="P54" s="38" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q54" s="39"/>
+      <c r="S54" s="38" t="s">
+        <v>343</v>
+      </c>
+      <c r="AMD54" s="42"/>
+      <c r="AME54" s="42"/>
+      <c r="AMF54" s="42"/>
+      <c r="AMG54" s="42"/>
+      <c r="AMH54" s="40"/>
+      <c r="AMI54" s="40"/>
+      <c r="AMJ54" s="40"/>
+    </row>
+    <row r="55" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="B55" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="K55" s="17" t="str">
         <f aca="false">IFERROR( ROUNDUP(B55*$O$79/J55,0), "" )</f>
         <v/>
       </c>
-      <c r="L55" s="0" t="n">
+      <c r="L55" s="17" t="n">
         <f aca="false">IF(J55&gt;0,J55*K55,$O$79)</f>
         <v>550</v>
       </c>
-      <c r="M55" s="3" t="e">
-        <f aca="false">8*L76</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N55" s="2" t="e">
+      <c r="M55" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" s="19" t="n">
         <f aca="false">L55*M55</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O55" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="P55" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q55" s="0" t="s">
-        <v>339</v>
+        <v>0</v>
+      </c>
+      <c r="O55" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="P55" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q55" s="17" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>343</v>
+        <v>353</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>354</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="K56" s="0" t="str">
+        <v>355</v>
+      </c>
+      <c r="J56" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K56" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B56*$O$79/J56,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L56" s="2" t="n">
         <f aca="false">IF(J56&gt;0,J56*K56,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M56" s="3" t="n">
-        <v>0.34</v>
+        <v>0.3287</v>
       </c>
       <c r="N56" s="2" t="n">
         <f aca="false">L56*M56</f>
-        <v>187</v>
+        <v>187.359</v>
       </c>
       <c r="O56" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P56" s="0" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="R56" s="13"/>
+      <c r="S56" s="0" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="K57" s="0" t="str">
+        <v>360</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="J57" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K57" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B57*$O$79/J57,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L57" s="2" t="n">
         <f aca="false">IF(J57&gt;0,J57*K57,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M57" s="3" t="n">
-        <v>0.98</v>
+        <v>0.77898</v>
       </c>
       <c r="N57" s="2" t="n">
         <f aca="false">L57*M57</f>
-        <v>539</v>
+        <v>444.0186</v>
       </c>
       <c r="O57" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P57" s="0" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>351</v>
+        <v>363</v>
+      </c>
+      <c r="S57" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>354</v>
+        <v>366</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>367</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="K58" s="0" t="str">
+        <v>368</v>
+      </c>
+      <c r="J58" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K58" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B58*$O$79/J58,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L58" s="2" t="n">
         <f aca="false">IF(J58&gt;0,J58*K58,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M58" s="3" t="n">
-        <v>0.54</v>
+        <v>1.12612</v>
       </c>
       <c r="N58" s="2" t="n">
         <f aca="false">L58*M58</f>
-        <v>297</v>
+        <v>641.8884</v>
       </c>
       <c r="O58" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P58" s="0" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>357</v>
+        <v>370</v>
+      </c>
+      <c r="S58" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>361</v>
+        <v>374</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>375</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="K59" s="0" t="str">
+        <v>376</v>
+      </c>
+      <c r="J59" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K59" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B59*$O$79/J59,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L59" s="2" t="n">
         <f aca="false">IF(J59&gt;0,J59*K59,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M59" s="3" t="n">
-        <v>0.095</v>
+        <v>0.20747</v>
       </c>
       <c r="N59" s="2" t="n">
         <f aca="false">L59*M59</f>
-        <v>52.25</v>
+        <v>118.2579</v>
       </c>
       <c r="O59" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P59" s="0" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>364</v>
+        <v>378</v>
+      </c>
+      <c r="S59" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>367</v>
+        <v>381</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>382</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="K60" s="0" t="str">
+        <v>383</v>
+      </c>
+      <c r="J60" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="K60" s="0" t="n">
         <f aca="false">IFERROR( ROUNDUP(B60*$O$79/J60,0), "" )</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L60" s="2" t="n">
         <f aca="false">IF(J60&gt;0,J60*K60,$O$79)</f>
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="M60" s="3" t="n">
-        <v>0.12</v>
+        <v>0.40872</v>
       </c>
       <c r="N60" s="2" t="n">
         <f aca="false">L60*M60</f>
-        <v>66</v>
+        <v>232.9704</v>
       </c>
       <c r="O60" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P60" s="0" t="s">
-        <v>369</v>
+        <v>384</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>370</v>
+        <v>385</v>
       </c>
       <c r="R60" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="S60" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D61" s="13"/>
-      <c r="E61" s="14"/>
+      <c r="E61" s="0"/>
       <c r="K61" s="0" t="str">
         <f aca="false">IFERROR( ROUNDUP(B61*$O$79/J61,0), "" )</f>
         <v/>
@@ -4877,111 +5132,117 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>371</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>372</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="J62" s="0"/>
-      <c r="K62" s="0" t="str">
+    <row r="62" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="B62" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" s="44" t="s">
+        <v>387</v>
+      </c>
+      <c r="E62" s="45" t="s">
+        <v>388</v>
+      </c>
+      <c r="F62" s="45" t="s">
+        <v>388</v>
+      </c>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="J62" s="44" t="n">
+        <v>570</v>
+      </c>
+      <c r="K62" s="44" t="n">
         <f aca="false">IFERROR( ROUNDUP(B62*$O$79/J62,0), "" )</f>
-        <v/>
-      </c>
-      <c r="L62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L62" s="44" t="n">
         <f aca="false">IF(J62&gt;0,J62*K62,$O$79)</f>
-        <v>550</v>
-      </c>
-      <c r="M62" s="3" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="N62" s="2" t="n">
+        <v>570</v>
+      </c>
+      <c r="M62" s="47" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="N62" s="48" t="n">
         <f aca="false">L62*M62</f>
-        <v>715</v>
-      </c>
-      <c r="O62" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P62" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q62" s="0"/>
-    </row>
-    <row r="63" s="31" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="31" t="s">
-        <v>376</v>
-      </c>
-      <c r="B63" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C63" s="32" t="s">
-        <v>372</v>
-      </c>
-      <c r="D63" s="31" t="s">
-        <v>377</v>
-      </c>
-      <c r="E63" s="32" t="s">
-        <v>378</v>
-      </c>
-      <c r="F63" s="0"/>
-      <c r="G63" s="0"/>
-      <c r="H63" s="0"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="34" t="str">
+        <v>1692.9</v>
+      </c>
+      <c r="O62" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="P62" s="44" t="s">
+        <v>389</v>
+      </c>
+      <c r="S62" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="AMI62" s="46"/>
+      <c r="AMJ62" s="46"/>
+    </row>
+    <row r="63" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="44" t="s">
+        <v>391</v>
+      </c>
+      <c r="B63" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="45"/>
+      <c r="D63" s="44" t="s">
+        <v>392</v>
+      </c>
+      <c r="E63" s="45" t="s">
+        <v>393</v>
+      </c>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="J63" s="48"/>
+      <c r="K63" s="49" t="str">
         <f aca="false">IFERROR( ROUNDUP(B63*$O$79/J63,0), "" )</f>
         <v/>
       </c>
-      <c r="L63" s="33" t="n">
+      <c r="L63" s="48" t="n">
         <f aca="false">IF(J63&gt;0,J63*K63,$O$79)</f>
         <v>550</v>
       </c>
-      <c r="M63" s="35" t="n">
+      <c r="M63" s="47" t="n">
         <v>3.1</v>
       </c>
-      <c r="N63" s="2" t="n">
+      <c r="N63" s="48" t="n">
         <f aca="false">L63*M63</f>
         <v>1705</v>
       </c>
-      <c r="O63" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="P63" s="31" t="s">
-        <v>379</v>
-      </c>
-      <c r="AMD63" s="34"/>
-      <c r="AME63" s="34"/>
-      <c r="AMF63" s="34"/>
-      <c r="AMG63" s="34"/>
-      <c r="AMH63" s="0"/>
-      <c r="AMI63" s="0"/>
-      <c r="AMJ63" s="0"/>
-    </row>
-    <row r="64" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="27" t="s">
-        <v>380</v>
-      </c>
-      <c r="B64" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C64" s="28" t="s">
-        <v>372</v>
-      </c>
-      <c r="E64" s="28"/>
-      <c r="F64" s="0"/>
-      <c r="G64" s="0"/>
-      <c r="H64" s="0"/>
+      <c r="O63" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="P63" s="44" t="s">
+        <v>394</v>
+      </c>
+      <c r="S63" s="44" t="s">
+        <v>395</v>
+      </c>
+      <c r="AMD63" s="49"/>
+      <c r="AME63" s="49"/>
+      <c r="AMF63" s="49"/>
+      <c r="AMG63" s="49"/>
+      <c r="AMI63" s="46"/>
+      <c r="AMJ63" s="46"/>
+    </row>
+    <row r="64" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="B64" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="28"/>
       <c r="J64" s="29"/>
-      <c r="K64" s="27" t="str">
+      <c r="K64" s="26" t="str">
         <f aca="false">IFERROR( ROUNDUP(B64*$O$79/J64,0), "" )</f>
         <v/>
       </c>
@@ -4992,207 +5253,220 @@
       <c r="M64" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="N64" s="2" t="n">
+      <c r="N64" s="29" t="n">
         <f aca="false">L64*M64</f>
         <v>550</v>
       </c>
-      <c r="AMH64" s="0"/>
-      <c r="AMI64" s="0"/>
-      <c r="AMJ64" s="0"/>
-    </row>
-    <row r="65" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="27" t="s">
-        <v>381</v>
-      </c>
-      <c r="B65" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C65" s="28" t="s">
-        <v>372</v>
-      </c>
-      <c r="D65" s="27" t="s">
-        <v>382</v>
-      </c>
-      <c r="E65" s="28"/>
-      <c r="F65" s="0"/>
-      <c r="G65" s="0"/>
-      <c r="H65" s="0"/>
-      <c r="J65" s="29"/>
-      <c r="K65" s="27" t="str">
+      <c r="S64" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="AMI64" s="28"/>
+      <c r="AMJ64" s="28"/>
+    </row>
+    <row r="65" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="44" t="s">
+        <v>398</v>
+      </c>
+      <c r="B65" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" s="45"/>
+      <c r="D65" s="44" t="s">
+        <v>399</v>
+      </c>
+      <c r="E65" s="45"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="46"/>
+      <c r="J65" s="48"/>
+      <c r="K65" s="44" t="str">
         <f aca="false">IFERROR( ROUNDUP(B65*$O$79/J65,0), "" )</f>
         <v/>
       </c>
-      <c r="L65" s="29" t="n">
+      <c r="L65" s="48" t="n">
         <f aca="false">IF(J65&gt;0,J65*K65,$O$79)</f>
         <v>550</v>
       </c>
-      <c r="M65" s="30" t="n">
+      <c r="M65" s="47" t="n">
         <v>0.6</v>
       </c>
-      <c r="N65" s="2" t="n">
+      <c r="N65" s="48" t="n">
         <f aca="false">L65*M65</f>
         <v>330</v>
       </c>
-      <c r="P65" s="27" t="s">
-        <v>383</v>
-      </c>
-      <c r="R65" s="27" t="s">
-        <v>308</v>
-      </c>
-      <c r="AMH65" s="0"/>
-      <c r="AMI65" s="0"/>
-      <c r="AMJ65" s="0"/>
-    </row>
-    <row r="66" s="31" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="31" t="s">
-        <v>384</v>
-      </c>
-      <c r="B66" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="0"/>
-      <c r="G66" s="0"/>
-      <c r="H66" s="0"/>
-      <c r="J66" s="33"/>
-      <c r="K66" s="34" t="str">
+      <c r="P65" s="44" t="s">
+        <v>400</v>
+      </c>
+      <c r="S65" s="44" t="s">
+        <v>401</v>
+      </c>
+      <c r="AMI65" s="46"/>
+      <c r="AMJ65" s="46"/>
+    </row>
+    <row r="66" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="B66" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" s="27"/>
+      <c r="D66" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="E66" s="27"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="28"/>
+      <c r="J66" s="29"/>
+      <c r="K66" s="50" t="str">
         <f aca="false">IFERROR( ROUNDUP(B66*$O$79/J66,0), "" )</f>
         <v/>
       </c>
-      <c r="L66" s="33" t="n">
+      <c r="L66" s="29" t="n">
         <f aca="false">IF(J66&gt;0,J66*K66,$O$79)</f>
         <v>550</v>
       </c>
-      <c r="M66" s="35"/>
-      <c r="N66" s="2" t="n">
+      <c r="M66" s="30"/>
+      <c r="N66" s="29" t="n">
         <f aca="false">L66*M66</f>
         <v>0</v>
       </c>
-      <c r="R66" s="34"/>
-      <c r="AMD66" s="34"/>
-      <c r="AME66" s="34"/>
-      <c r="AMF66" s="34"/>
-      <c r="AMG66" s="34"/>
-      <c r="AMH66" s="0"/>
-      <c r="AMI66" s="0"/>
-      <c r="AMJ66" s="0"/>
-    </row>
-    <row r="67" s="31" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="31" t="s">
-        <v>385</v>
-      </c>
-      <c r="B67" s="31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C67" s="32"/>
-      <c r="D67" s="31" t="s">
-        <v>386</v>
-      </c>
-      <c r="E67" s="32" t="s">
-        <v>387</v>
-      </c>
-      <c r="F67" s="0"/>
-      <c r="G67" s="0"/>
-      <c r="H67" s="0"/>
-      <c r="J67" s="33" t="n">
+      <c r="R66" s="50"/>
+      <c r="S66" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="AMD66" s="50"/>
+      <c r="AME66" s="50"/>
+      <c r="AMF66" s="50"/>
+      <c r="AMG66" s="50"/>
+      <c r="AMI66" s="28"/>
+      <c r="AMJ66" s="28"/>
+    </row>
+    <row r="67" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="B67" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" s="27"/>
+      <c r="D67" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
+      <c r="J67" s="29" t="n">
         <v>600</v>
       </c>
-      <c r="K67" s="34" t="n">
+      <c r="K67" s="50" t="n">
         <f aca="false">IFERROR( ROUNDUP(B67*$O$79/J67,0), "" )</f>
         <v>1</v>
       </c>
-      <c r="L67" s="33" t="n">
+      <c r="L67" s="29" t="n">
         <f aca="false">IF(J67&gt;0,J67*K67,$O$79)</f>
         <v>600</v>
       </c>
-      <c r="M67" s="35"/>
-      <c r="N67" s="2" t="n">
+      <c r="M67" s="30"/>
+      <c r="N67" s="29" t="n">
         <f aca="false">L67*M67</f>
         <v>0</v>
       </c>
-      <c r="R67" s="34"/>
-      <c r="AMD67" s="34"/>
-      <c r="AME67" s="34"/>
-      <c r="AMF67" s="34"/>
-      <c r="AMG67" s="34"/>
-      <c r="AMH67" s="0"/>
-      <c r="AMI67" s="0"/>
-      <c r="AMJ67" s="0"/>
-    </row>
-    <row r="68" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="B68" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="0"/>
-      <c r="G68" s="0"/>
-      <c r="H68" s="0"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="19"/>
-      <c r="K68" s="36" t="str">
+      <c r="R67" s="50"/>
+      <c r="S67" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="AMD67" s="50"/>
+      <c r="AME67" s="50"/>
+      <c r="AMF67" s="50"/>
+      <c r="AMG67" s="50"/>
+      <c r="AMI67" s="28"/>
+      <c r="AMJ67" s="28"/>
+    </row>
+    <row r="68" s="50" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="26" t="s">
+        <v>406</v>
+      </c>
+      <c r="B68" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" s="27"/>
+      <c r="D68" s="26" t="s">
+        <v>407</v>
+      </c>
+      <c r="E68" s="27"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="28"/>
+      <c r="H68" s="28"/>
+      <c r="I68" s="26"/>
+      <c r="J68" s="29"/>
+      <c r="K68" s="50" t="str">
         <f aca="false">IFERROR( ROUNDUP(B68*$O$79/J68,0), "" )</f>
         <v/>
       </c>
-      <c r="L68" s="19" t="n">
+      <c r="L68" s="29" t="n">
         <f aca="false">IF(J68&gt;0,J68*K68,$O$79)</f>
         <v>550</v>
       </c>
-      <c r="M68" s="20"/>
-      <c r="N68" s="2" t="n">
+      <c r="M68" s="30"/>
+      <c r="N68" s="29" t="n">
         <f aca="false">L68*M68</f>
         <v>0</v>
       </c>
-      <c r="O68" s="17"/>
-      <c r="P68" s="17"/>
-      <c r="Q68" s="18"/>
-      <c r="R68" s="17"/>
-      <c r="T68" s="17"/>
-      <c r="AMH68" s="0"/>
-      <c r="AMI68" s="0"/>
-      <c r="AMJ68" s="0"/>
-    </row>
-    <row r="69" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="17" t="s">
-        <v>389</v>
-      </c>
-      <c r="B69" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C69" s="18"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="0"/>
-      <c r="G69" s="0"/>
-      <c r="H69" s="0"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="19"/>
-      <c r="K69" s="36" t="str">
+      <c r="O68" s="26"/>
+      <c r="P68" s="26"/>
+      <c r="Q68" s="27"/>
+      <c r="R68" s="26"/>
+      <c r="S68" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="T68" s="26"/>
+      <c r="AMH68" s="26"/>
+      <c r="AMI68" s="28"/>
+      <c r="AMJ68" s="28"/>
+    </row>
+    <row r="69" s="49" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="44" t="s">
+        <v>409</v>
+      </c>
+      <c r="B69" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" s="45"/>
+      <c r="D69" s="44" t="s">
+        <v>410</v>
+      </c>
+      <c r="E69" s="45"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
+      <c r="I69" s="44"/>
+      <c r="J69" s="48"/>
+      <c r="K69" s="49" t="str">
         <f aca="false">IFERROR( ROUNDUP(B69*$O$79/J69,0), "" )</f>
         <v/>
       </c>
-      <c r="L69" s="19" t="n">
+      <c r="L69" s="48" t="n">
         <f aca="false">IF(J69&gt;0,J69*K69,$O$79)</f>
         <v>550</v>
       </c>
-      <c r="M69" s="20"/>
-      <c r="N69" s="2" t="n">
+      <c r="M69" s="47"/>
+      <c r="N69" s="48" t="n">
         <f aca="false">L69*M69</f>
         <v>0</v>
       </c>
-      <c r="O69" s="17"/>
-      <c r="P69" s="17"/>
-      <c r="Q69" s="18"/>
-      <c r="R69" s="17"/>
-      <c r="T69" s="17"/>
-      <c r="AMH69" s="0"/>
-      <c r="AMI69" s="0"/>
-      <c r="AMJ69" s="0"/>
+      <c r="O69" s="44"/>
+      <c r="P69" s="44"/>
+      <c r="Q69" s="45"/>
+      <c r="R69" s="44"/>
+      <c r="S69" s="44" t="s">
+        <v>411</v>
+      </c>
+      <c r="T69" s="44"/>
+      <c r="AMH69" s="44"/>
+      <c r="AMI69" s="46"/>
+      <c r="AMJ69" s="46"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K70" s="0"/>
@@ -5202,86 +5476,99 @@
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
       <c r="M72" s="7" t="s">
-        <v>390</v>
-      </c>
-      <c r="N72" s="6" t="e">
+        <v>412</v>
+      </c>
+      <c r="N72" s="6" t="n">
         <f aca="false">SUM(N2:N71)</f>
-        <v>#VALUE!</v>
+        <v>21395.5026</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L73" s="6"/>
       <c r="M73" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="N73" s="6" t="e">
+        <v>413</v>
+      </c>
+      <c r="N73" s="6" t="n">
         <f aca="false">N72/$O$79</f>
-        <v>#VALUE!</v>
+        <v>38.9009138181818</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>392</v>
-      </c>
-      <c r="B74" s="0" t="n">
+      <c r="A74" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B74" s="4" t="n">
         <f aca="false">SUM(B2:B73)</f>
         <v>178</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O75" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P75" s="0" t="s">
-        <v>393</v>
+        <v>415</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L76" s="6" t="s">
-        <v>394</v>
+        <v>416</v>
       </c>
       <c r="O76" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P76" s="0" t="s">
-        <v>395</v>
+        <v>417</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O77" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="P77" s="0" t="s">
-        <v>396</v>
-      </c>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="51" t="s">
+        <v>419</v>
+      </c>
+      <c r="D78" s="52"/>
+      <c r="E78" s="53"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="54" t="s">
+        <v>420</v>
+      </c>
       <c r="O79" s="4" t="n">
         <v>550</v>
       </c>
       <c r="P79" s="0" t="s">
-        <v>397</v>
+        <v>421</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="37" t="s">
-        <v>398</v>
+      <c r="A80" s="55" t="s">
+        <v>422</v>
       </c>
       <c r="C80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="38" t="s">
-        <v>399</v>
+      <c r="A81" s="56" t="s">
+        <v>423</v>
       </c>
       <c r="C81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="39" t="s">
-        <v>400</v>
+      <c r="A82" s="57" t="s">
+        <v>424</v>
       </c>
       <c r="C82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="58" t="s">
+        <v>425</v>
+      </c>
       <c r="O83" s="14"/>
       <c r="P83" s="13"/>
     </row>

</xml_diff>

<commit_message>
Remove space-wasting column, add some TODO's
</commit_message>
<xml_diff>
--- a/r2/bom/tr20-r2-alternative-sources.xlsx
+++ b/r2/bom/tr20-r2-alternative-sources.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="420">
   <si>
     <t xml:space="preserve">References</t>
   </si>
@@ -64,9 +64,6 @@
     <t xml:space="preserve">Line GBP</t>
   </si>
   <si>
-    <t xml:space="preserve">Substitute</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t xml:space="preserve">C162143</t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
     <t xml:space="preserve">U2J, 1.5nF, 10V, -5%/+5%</t>
   </si>
   <si>
@@ -364,9 +358,6 @@
     <t xml:space="preserve">C261278 </t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bidirectional transient-voltage-suppression diode 6V</t>
   </si>
   <si>
@@ -622,9 +613,6 @@
     <t xml:space="preserve">C184029 </t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
     <t xml:space="preserve">Inductor</t>
   </si>
   <si>
@@ -1129,7 +1117,7 @@
     <t xml:space="preserve">C131154</t>
   </si>
   <si>
-    <t xml:space="preserve">2VRMS DirectPath, 100dB Audio Stereo DAC with 32-bit, 384kHz PCM Interface, TSSOP-20</t>
+    <t xml:space="preserve">2VRMS DirectPath, 100dB Audio Stereo DAC</t>
   </si>
   <si>
     <t xml:space="preserve">TSSOP-20_4.4x6.5mm_P0.65mm</t>
@@ -1258,7 +1246,7 @@
     <t xml:space="preserve">Need components from around 22/2</t>
   </si>
   <si>
-    <t xml:space="preserve">Total</t>
+    <t xml:space="preserve">Total GBP</t>
   </si>
   <si>
     <t xml:space="preserve">Unit</t>
@@ -1267,22 +1255,16 @@
     <t xml:space="preserve">Total parts</t>
   </si>
   <si>
-    <t xml:space="preserve">Substitution OK</t>
-  </si>
-  <si>
     <t xml:space="preserve">Exchange</t>
   </si>
   <si>
-    <t xml:space="preserve">Check before substituting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do not substitute</t>
-  </si>
-  <si>
     <t xml:space="preserve">TODO: compare against tr20-r2.xlsx – missing the 5.1k resistors. Is something else missing ?</t>
   </si>
   <si>
     <t xml:space="preserve">Happy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">also add a “surplus” column to calculate how many extra parts we have for each line, as a sanity check</t>
   </si>
   <si>
     <t xml:space="preserve">Units to build</t>
@@ -1956,8 +1938,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F45" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I72" activeCellId="0" sqref="I72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C80" activeCellId="0" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1976,10 +1958,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="46.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="47.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="52.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="24.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="78.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="34.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="41.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
@@ -2031,18 +2013,16 @@
       <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="AMC1" s="0"/>
       <c r="AMD1" s="0"/>
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
@@ -2053,25 +2033,25 @@
     </row>
     <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="E2" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="8" t="str">
@@ -2089,36 +2069,37 @@
         <f aca="false">L2*M2</f>
         <v>2310</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="P2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="AMH2" s="10"/>
       <c r="AMI2" s="10"/>
-      <c r="AMJ2" s="10"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="I3" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>600</v>
@@ -2138,37 +2119,34 @@
         <f aca="false">L3*M3</f>
         <v>90</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="Q3" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="13" t="n">
         <v>15</v>
       </c>
       <c r="C4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="F4" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
@@ -2190,9 +2168,10 @@
         <f aca="false">L4*M4</f>
         <v>33.5</v>
       </c>
-      <c r="Q4" s="14" t="s">
-        <v>33</v>
-      </c>
+      <c r="P4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AMC4" s="0"/>
       <c r="AMD4" s="0"/>
       <c r="AME4" s="0"/>
       <c r="AMF4" s="0"/>
@@ -2203,22 +2182,22 @@
     </row>
     <row r="5" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="13" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="G5" s="0"/>
       <c r="H5" s="0"/>
@@ -2240,15 +2219,16 @@
         <f aca="false">L5*M5</f>
         <v>44.8</v>
       </c>
+      <c r="O5" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="P5" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC5" s="0"/>
       <c r="AMD5" s="0"/>
       <c r="AME5" s="0"/>
       <c r="AMF5" s="0"/>
@@ -2259,22 +2239,22 @@
     </row>
     <row r="6" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="G6" s="0"/>
       <c r="H6" s="0"/>
@@ -2296,12 +2276,13 @@
         <f aca="false">L6*M6</f>
         <v>27.4</v>
       </c>
+      <c r="O6" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="P6" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="AMC6" s="0"/>
       <c r="AMD6" s="0"/>
       <c r="AME6" s="0"/>
       <c r="AMF6" s="0"/>
@@ -2312,22 +2293,22 @@
     </row>
     <row r="7" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="13" t="n">
         <v>5</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
@@ -2349,15 +2330,16 @@
         <f aca="false">L7*M7</f>
         <v>44.9</v>
       </c>
+      <c r="O7" s="14" t="s">
+        <v>53</v>
+      </c>
       <c r="P7" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC7" s="0"/>
       <c r="AMD7" s="0"/>
       <c r="AME7" s="0"/>
       <c r="AMF7" s="0"/>
@@ -2368,22 +2350,22 @@
     </row>
     <row r="8" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>59</v>
       </c>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
@@ -2405,15 +2387,16 @@
         <f aca="false">L8*M8</f>
         <v>70.6</v>
       </c>
+      <c r="O8" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="P8" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q8" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC8" s="0"/>
       <c r="AMD8" s="0"/>
       <c r="AME8" s="0"/>
       <c r="AMF8" s="0"/>
@@ -2424,22 +2407,22 @@
     </row>
     <row r="9" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" s="13" t="n">
         <v>23</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
@@ -2461,15 +2444,16 @@
         <f aca="false">L9*M9</f>
         <v>263.68</v>
       </c>
-      <c r="P9" s="13" t="s">
+      <c r="O9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q9" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="R9" s="13" t="s">
-        <v>67</v>
-      </c>
+      <c r="AMC9" s="0"/>
       <c r="AMD9" s="0"/>
       <c r="AME9" s="0"/>
       <c r="AMF9" s="0"/>
@@ -2480,22 +2464,22 @@
     </row>
     <row r="10" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="14" t="s">
+      <c r="F10" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
@@ -2517,15 +2501,16 @@
         <f aca="false">L10*M10</f>
         <v>44.8</v>
       </c>
+      <c r="O10" s="14" t="s">
+        <v>70</v>
+      </c>
       <c r="P10" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R10" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC10" s="0"/>
       <c r="AMD10" s="0"/>
       <c r="AME10" s="0"/>
       <c r="AMF10" s="0"/>
@@ -2536,22 +2521,22 @@
     </row>
     <row r="11" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="14" t="s">
+      <c r="F11" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
@@ -2573,12 +2558,13 @@
         <f aca="false">L11*M11</f>
         <v>87.4</v>
       </c>
+      <c r="O11" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="P11" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="AMC11" s="0"/>
       <c r="AMD11" s="0"/>
       <c r="AME11" s="0"/>
       <c r="AMF11" s="0"/>
@@ -2589,22 +2575,22 @@
     </row>
     <row r="12" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C12" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>81</v>
       </c>
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
@@ -2626,12 +2612,13 @@
         <f aca="false">L12*M12</f>
         <v>406.02</v>
       </c>
-      <c r="P12" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q12" s="14" t="s">
-        <v>66</v>
-      </c>
+      <c r="O12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AMC12" s="0"/>
       <c r="AMD12" s="0"/>
       <c r="AME12" s="0"/>
       <c r="AMF12" s="0"/>
@@ -2642,22 +2629,22 @@
     </row>
     <row r="13" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B13" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
@@ -2679,15 +2666,16 @@
         <f aca="false">L13*M13</f>
         <v>122.2</v>
       </c>
+      <c r="O13" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="P13" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q13" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R13" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC13" s="0"/>
       <c r="AMD13" s="0"/>
       <c r="AME13" s="0"/>
       <c r="AMF13" s="0"/>
@@ -2698,22 +2686,22 @@
     </row>
     <row r="14" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="F14" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
@@ -2735,15 +2723,16 @@
         <f aca="false">L14*M14</f>
         <v>44.6</v>
       </c>
+      <c r="O14" s="14" t="s">
+        <v>90</v>
+      </c>
       <c r="P14" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R14" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC14" s="0"/>
       <c r="AMD14" s="0"/>
       <c r="AME14" s="0"/>
       <c r="AMF14" s="0"/>
@@ -2754,22 +2743,22 @@
     </row>
     <row r="15" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="14" t="s">
+      <c r="F15" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
@@ -2791,15 +2780,16 @@
         <f aca="false">L15*M15</f>
         <v>70.6</v>
       </c>
+      <c r="O15" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="P15" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q15" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R15" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="Q15" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC15" s="0"/>
       <c r="AMD15" s="0"/>
       <c r="AME15" s="0"/>
       <c r="AMF15" s="0"/>
@@ -2810,22 +2800,22 @@
     </row>
     <row r="16" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B16" s="13" t="n">
         <v>2</v>
       </c>
       <c r="C16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
@@ -2847,15 +2837,16 @@
         <f aca="false">L16*M16</f>
         <v>149.56</v>
       </c>
-      <c r="P16" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q16" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="R16" s="13" t="s">
-        <v>67</v>
-      </c>
+      <c r="O16" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q16" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AMC16" s="0"/>
       <c r="AMD16" s="0"/>
       <c r="AME16" s="0"/>
       <c r="AMF16" s="0"/>
@@ -2866,22 +2857,22 @@
     </row>
     <row r="17" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B17" s="13" t="n">
         <v>11</v>
       </c>
       <c r="C17" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
@@ -2903,15 +2894,16 @@
         <f aca="false">L17*M17</f>
         <v>80.2</v>
       </c>
+      <c r="O17" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="P17" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q17" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R17" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="Q17" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC17" s="0"/>
       <c r="AMD17" s="0"/>
       <c r="AME17" s="0"/>
       <c r="AMF17" s="0"/>
@@ -2922,25 +2914,25 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="I18" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="J18" s="2" t="n">
         <v>8000</v>
@@ -2961,36 +2953,34 @@
         <v>201.68</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P18" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q18" s="0"/>
     </row>
     <row r="19" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="F19" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="I19" s="17" t="s">
         <v>119</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>122</v>
       </c>
       <c r="J19" s="19" t="n">
         <v>600</v>
@@ -3011,39 +3001,37 @@
         <v>43.338</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="P19" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q19" s="18" t="n">
+        <v>120</v>
+      </c>
+      <c r="P19" s="18" t="n">
         <v>1206</v>
       </c>
-      <c r="S19" s="17" t="s">
-        <v>124</v>
-      </c>
+      <c r="R19" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="I20" s="13" t="s">
         <v>126</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>129</v>
       </c>
       <c r="J20" s="2" t="n">
         <v>3000</v>
@@ -3063,39 +3051,37 @@
         <v>43.338</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P20" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q20" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="P20" s="1" t="n">
         <v>1206</v>
       </c>
-      <c r="S20" s="0" t="s">
-        <v>131</v>
+      <c r="Q20" s="0"/>
+      <c r="R20" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I21" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>136</v>
       </c>
       <c r="J21" s="2" t="n">
         <v>3000</v>
@@ -3116,36 +3102,34 @@
         <v>143.37</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P21" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>138</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J22" s="2" t="n">
         <v>3000</v>
@@ -3165,33 +3149,31 @@
         <v>43.338</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P22" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q22" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="P22" s="1" t="n">
         <v>1206</v>
       </c>
-      <c r="S22" s="0" t="s">
-        <v>131</v>
+      <c r="Q22" s="0"/>
+      <c r="R22" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="23" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B23" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
@@ -3209,21 +3191,19 @@
         <f aca="false">L23*M23</f>
         <v>0</v>
       </c>
-      <c r="O23" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q23" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="S23" s="21" t="s">
-        <v>147</v>
-      </c>
+      <c r="P23" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="R23" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="AMH23" s="23"/>
       <c r="AMI23" s="23"/>
-      <c r="AMJ23" s="23"/>
+      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>2</v>
@@ -3232,16 +3212,16 @@
         <v>532610271</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E24" s="1" t="n">
         <v>532610271</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>1200</v>
@@ -3261,37 +3241,35 @@
         <f aca="false">L24*M24</f>
         <v>223.2</v>
       </c>
-      <c r="O24" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="S24" s="0" t="s">
-        <v>153</v>
+      <c r="P24" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q24" s="0"/>
+      <c r="R24" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="B25" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="13" t="s">
+      <c r="I25" s="13" t="s">
         <v>155</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="J25" s="2" t="n">
         <v>600</v>
@@ -3312,38 +3290,36 @@
         <v>294</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P25" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>160</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q25" s="0"/>
     </row>
     <row r="26" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="B26" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>164</v>
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="0"/>
       <c r="I26" s="13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J26" s="16" t="n">
         <v>570</v>
@@ -3363,12 +3339,10 @@
         <f aca="false">L26*M26</f>
         <v>864.519</v>
       </c>
-      <c r="O26" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q26" s="14" t="s">
-        <v>166</v>
-      </c>
+      <c r="P26" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="AMC26" s="0"/>
       <c r="AMD26" s="0"/>
       <c r="AME26" s="0"/>
       <c r="AMF26" s="0"/>
@@ -3379,25 +3353,25 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="I27" s="13" t="s">
         <v>168</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>171</v>
       </c>
       <c r="J27" s="2" t="n">
         <v>570</v>
@@ -3418,36 +3392,34 @@
         <v>315.5064</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P27" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>173</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H28" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="B28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="I28" s="13" t="s">
         <v>175</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>178</v>
       </c>
       <c r="J28" s="2" t="n">
         <v>1000</v>
@@ -3468,36 +3440,34 @@
         <v>570</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P28" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>180</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E29" s="1" t="n">
         <v>629104190121</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>570</v>
@@ -3518,36 +3488,34 @@
         <v>442.4283</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>31</v>
+        <v>183</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q29" s="0" t="s">
-        <v>187</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="Q29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="I30" s="13" t="s">
         <v>189</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>192</v>
       </c>
       <c r="J30" s="2" t="n">
         <v>570</v>
@@ -3568,36 +3536,34 @@
         <v>432.63</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P30" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>194</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F31" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="B31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="I31" s="13" t="s">
         <v>196</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>199</v>
       </c>
       <c r="J31" s="2" t="n">
         <v>600</v>
@@ -3618,42 +3584,39 @@
         <v>44.04</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="P31" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="R31" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="S31" s="0" t="s">
-        <v>131</v>
+        <v>197</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q31" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F32" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="B32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="I32" s="13" t="s">
         <v>204</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>208</v>
       </c>
       <c r="J32" s="2" t="n">
         <v>570</v>
@@ -3674,36 +3637,34 @@
         <v>71.2215</v>
       </c>
       <c r="O32" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P32" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>210</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="J33" s="2" t="n">
         <v>3000</v>
@@ -3724,42 +3685,39 @@
         <v>146.82</v>
       </c>
       <c r="O33" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="P33" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="R33" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="S33" s="0" t="s">
-        <v>131</v>
+        <v>197</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="R33" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="I34" s="13" t="s">
         <v>216</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>220</v>
       </c>
       <c r="J34" s="2" t="n">
         <v>600</v>
@@ -3780,42 +3738,39 @@
         <v>44.04</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="P34" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="R34" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="S34" s="0" t="s">
-        <v>131</v>
+        <v>197</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q34" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="R34" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="I35" s="13" t="s">
         <v>221</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="I35" s="13" t="s">
-        <v>225</v>
       </c>
       <c r="J35" s="2" t="n">
         <v>600</v>
@@ -3836,42 +3791,39 @@
         <v>44.04</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="P35" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="R35" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="S35" s="0" t="s">
-        <v>131</v>
+        <v>197</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q35" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="R35" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="I36" s="13" t="s">
         <v>226</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>230</v>
       </c>
       <c r="J36" s="2" t="n">
         <v>600</v>
@@ -3892,38 +3844,35 @@
         <v>47.988</v>
       </c>
       <c r="O36" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="P36" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="R36" s="13" t="s">
-        <v>45</v>
+        <v>197</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q36" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="37" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="26" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B37" s="26" t="n">
         <v>6</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F37" s="28"/>
       <c r="G37" s="28"/>
       <c r="H37" s="28" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="I37" s="26" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="J37" s="29" t="n">
         <v>900</v>
@@ -3944,41 +3893,39 @@
         <v>353.88</v>
       </c>
       <c r="O37" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="P37" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="Q37" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="S37" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="AMI37" s="28"/>
+        <v>232</v>
+      </c>
+      <c r="P37" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="R37" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="AMH37" s="28"/>
+      <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="J38" s="2" t="n">
         <v>1200</v>
@@ -3999,39 +3946,37 @@
         <v>72.804</v>
       </c>
       <c r="O38" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P38" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="S38" s="0" t="s">
-        <v>131</v>
+        <v>240</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q38" s="0"/>
+      <c r="R38" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J39" s="2" t="n">
         <v>3000</v>
@@ -4052,36 +3997,34 @@
         <v>54.03</v>
       </c>
       <c r="O39" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P39" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>245</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="I40" s="0" t="s">
         <v>252</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>256</v>
       </c>
       <c r="J40" s="2" t="n">
         <v>570</v>
@@ -4102,33 +4045,31 @@
         <v>57.342</v>
       </c>
       <c r="O40" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P40" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>258</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>259</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>263</v>
       </c>
       <c r="J41" s="0" t="n">
         <v>10000</v>
@@ -4148,31 +4089,32 @@
         <f aca="false">L41*M41</f>
         <v>10.2</v>
       </c>
+      <c r="O41" s="0" t="s">
+        <v>260</v>
+      </c>
       <c r="P41" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q41" s="0" t="s">
-        <v>265</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="Q41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>10000</v>
@@ -4192,31 +4134,32 @@
         <f aca="false">L42*M42</f>
         <v>18.8</v>
       </c>
-      <c r="P42" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>265</v>
-      </c>
+      <c r="O42" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>17</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>10000</v>
@@ -4236,31 +4179,32 @@
         <f aca="false">L43*M43</f>
         <v>12.5</v>
       </c>
-      <c r="P43" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>265</v>
-      </c>
+      <c r="O43" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>10000</v>
@@ -4280,31 +4224,32 @@
         <f aca="false">L44*M44</f>
         <v>12.5</v>
       </c>
-      <c r="P44" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>265</v>
-      </c>
+      <c r="O44" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="J45" s="0" t="n">
         <v>10000</v>
@@ -4324,31 +4269,32 @@
         <f aca="false">L45*M45</f>
         <v>18.8</v>
       </c>
-      <c r="P45" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>265</v>
-      </c>
+      <c r="O45" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="J46" s="0" t="n">
         <v>10000</v>
@@ -4368,38 +4314,39 @@
         <f aca="false">L46*M46</f>
         <v>12.5</v>
       </c>
-      <c r="P46" s="31" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q46" s="1" t="s">
-        <v>265</v>
-      </c>
+      <c r="O46" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q46" s="0"/>
     </row>
     <row r="47" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="B47" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="F47" s="0" t="s">
         <v>288</v>
-      </c>
-      <c r="B47" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>292</v>
       </c>
       <c r="G47" s="0"/>
       <c r="H47" s="13" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="J47" s="2" t="n">
         <v>570</v>
@@ -4420,17 +4367,15 @@
         <v>387.6</v>
       </c>
       <c r="O47" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="P47" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q47" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="S47" s="13" t="s">
-        <v>296</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="P47" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="R47" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="AMC47" s="0"/>
       <c r="AMD47" s="0"/>
       <c r="AME47" s="0"/>
       <c r="AMF47" s="0"/>
@@ -4441,25 +4386,25 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="I48" s="0" t="s">
         <v>297</v>
-      </c>
-      <c r="B48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="I48" s="0" t="s">
-        <v>301</v>
       </c>
       <c r="J48" s="2" t="n">
         <v>570</v>
@@ -4480,39 +4425,37 @@
         <v>207.8619</v>
       </c>
       <c r="O48" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P48" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="S48" s="0" t="s">
-        <v>131</v>
+        <v>298</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q48" s="0"/>
+      <c r="R48" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C49" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="I49" s="0" t="s">
         <v>305</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="I49" s="0" t="s">
-        <v>309</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>1000</v>
@@ -4533,36 +4476,34 @@
         <v>321.84</v>
       </c>
       <c r="O49" s="0" t="s">
-        <v>114</v>
+        <v>306</v>
       </c>
       <c r="P49" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q49" s="0" t="s">
-        <v>311</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="Q49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F50" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="B50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="I50" s="13" t="s">
         <v>313</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>317</v>
       </c>
       <c r="J50" s="2" t="n">
         <v>570</v>
@@ -4583,36 +4524,34 @@
         <v>64.7691</v>
       </c>
       <c r="O50" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P50" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q50" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="S50" s="0" t="s">
-        <v>131</v>
+        <v>314</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q50" s="0"/>
+      <c r="R50" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F51" s="0" t="s">
         <v>320</v>
-      </c>
-      <c r="B51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>324</v>
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="2" t="n">
@@ -4634,37 +4573,34 @@
         <v>1407.0222</v>
       </c>
       <c r="O51" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="P51" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="R51" s="13"/>
-      <c r="S51" s="0" t="s">
-        <v>131</v>
+        <v>321</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="I52" s="13"/>
       <c r="J52" s="2" t="n">
@@ -4686,36 +4622,34 @@
         <v>550.6713</v>
       </c>
       <c r="O52" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P52" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="S52" s="0" t="s">
-        <v>131</v>
+        <v>327</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q52" s="0"/>
+      <c r="R52" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="53" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="32" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B53" s="32" t="n">
         <v>1</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F53" s="32" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G53" s="32"/>
       <c r="H53" s="32"/>
@@ -4739,38 +4673,36 @@
         <v>724.2306</v>
       </c>
       <c r="O53" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="P53" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q53" s="33" t="s">
-        <v>338</v>
-      </c>
-      <c r="R53" s="32"/>
-      <c r="S53" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="T53" s="32"/>
-      <c r="AMH53" s="37"/>
+        <v>333</v>
+      </c>
+      <c r="P53" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q53" s="32"/>
+      <c r="R53" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="S53" s="32"/>
+      <c r="AMG53" s="37"/>
+      <c r="AMH53" s="32"/>
       <c r="AMI53" s="32"/>
-      <c r="AMJ53" s="32"/>
+      <c r="AMJ53" s="0"/>
     </row>
     <row r="54" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="38" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B54" s="38" t="n">
         <v>1</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F54" s="40"/>
       <c r="G54" s="40"/>
@@ -4792,38 +4724,36 @@
         <v>3300</v>
       </c>
       <c r="O54" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="P54" s="38" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q54" s="39"/>
-      <c r="S54" s="38" t="s">
-        <v>343</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="P54" s="39"/>
+      <c r="R54" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="AMC54" s="42"/>
       <c r="AMD54" s="42"/>
       <c r="AME54" s="42"/>
       <c r="AMF54" s="42"/>
-      <c r="AMG54" s="42"/>
+      <c r="AMG54" s="40"/>
       <c r="AMH54" s="40"/>
       <c r="AMI54" s="40"/>
-      <c r="AMJ54" s="40"/>
+      <c r="AMJ54" s="0"/>
     </row>
     <row r="55" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="17" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B55" s="17" t="n">
         <v>1</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="K55" s="17" t="str">
         <f aca="false">IFERROR( ROUNDUP(B55*$O$79/J55,0), "" )</f>
@@ -4841,36 +4771,34 @@
         <v>0</v>
       </c>
       <c r="O55" s="17" t="s">
-        <v>200</v>
+        <v>344</v>
       </c>
       <c r="P55" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="Q55" s="17" t="s">
-        <v>349</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="AMJ55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F56" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="B56" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="I56" s="0" t="s">
         <v>351</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="I56" s="0" t="s">
-        <v>355</v>
       </c>
       <c r="J56" s="2" t="n">
         <v>570</v>
@@ -4891,37 +4819,34 @@
         <v>187.359</v>
       </c>
       <c r="O56" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P56" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="R56" s="13"/>
-      <c r="S56" s="0" t="s">
-        <v>131</v>
+        <v>352</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q56" s="13"/>
+      <c r="R56" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="J57" s="2" t="n">
         <v>570</v>
@@ -4942,39 +4867,37 @@
         <v>444.0186</v>
       </c>
       <c r="O57" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P57" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="S57" s="0" t="s">
-        <v>131</v>
+        <v>358</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q57" s="0"/>
+      <c r="R57" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="I58" s="0" t="s">
         <v>364</v>
-      </c>
-      <c r="B58" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="F58" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="I58" s="0" t="s">
-        <v>368</v>
       </c>
       <c r="J58" s="2" t="n">
         <v>570</v>
@@ -4995,39 +4918,37 @@
         <v>641.8884</v>
       </c>
       <c r="O58" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P58" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="Q58" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="S58" s="0" t="s">
-        <v>131</v>
+        <v>365</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q58" s="0"/>
+      <c r="R58" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="F59" s="0" t="s">
         <v>371</v>
       </c>
-      <c r="B59" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="I59" s="0" t="s">
         <v>372</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>373</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="F59" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="I59" s="0" t="s">
-        <v>376</v>
       </c>
       <c r="J59" s="2" t="n">
         <v>570</v>
@@ -5048,39 +4969,37 @@
         <v>118.2579</v>
       </c>
       <c r="O59" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P59" s="0" t="s">
-        <v>377</v>
-      </c>
-      <c r="Q59" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="S59" s="0" t="s">
-        <v>131</v>
+        <v>373</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q59" s="0"/>
+      <c r="R59" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="I60" s="0" t="s">
         <v>379</v>
-      </c>
-      <c r="B60" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>382</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>383</v>
       </c>
       <c r="J60" s="2" t="n">
         <v>570</v>
@@ -5101,19 +5020,16 @@
         <v>232.9704</v>
       </c>
       <c r="O60" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P60" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="Q60" s="1" t="s">
-        <v>385</v>
+        <v>380</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q60" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="R60" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="S60" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5131,22 +5047,24 @@
         <f aca="false">L61*M61</f>
         <v>0</v>
       </c>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="0"/>
     </row>
     <row r="62" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="44" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B62" s="44" t="n">
         <v>1</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E62" s="45" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F62" s="45" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="G62" s="46"/>
       <c r="H62" s="46"/>
@@ -5169,30 +5087,28 @@
         <v>1692.9</v>
       </c>
       <c r="O62" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="P62" s="44" t="s">
-        <v>389</v>
-      </c>
-      <c r="S62" s="44" t="s">
-        <v>390</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="R62" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="AMH62" s="46"/>
       <c r="AMI62" s="46"/>
-      <c r="AMJ62" s="46"/>
+      <c r="AMJ62" s="0"/>
     </row>
     <row r="63" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="44" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B63" s="44" t="n">
         <v>1</v>
       </c>
       <c r="C63" s="45"/>
       <c r="D63" s="44" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E63" s="45" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F63" s="46"/>
       <c r="G63" s="46"/>
@@ -5214,24 +5130,22 @@
         <v>1705</v>
       </c>
       <c r="O63" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="P63" s="44" t="s">
-        <v>394</v>
-      </c>
-      <c r="S63" s="44" t="s">
-        <v>395</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="R63" s="44" t="s">
+        <v>391</v>
+      </c>
+      <c r="AMC63" s="49"/>
       <c r="AMD63" s="49"/>
       <c r="AME63" s="49"/>
       <c r="AMF63" s="49"/>
-      <c r="AMG63" s="49"/>
+      <c r="AMH63" s="46"/>
       <c r="AMI63" s="46"/>
-      <c r="AMJ63" s="46"/>
+      <c r="AMJ63" s="0"/>
     </row>
     <row r="64" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="26" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B64" s="26" t="n">
         <v>1</v>
@@ -5257,22 +5171,23 @@
         <f aca="false">L64*M64</f>
         <v>550</v>
       </c>
-      <c r="S64" s="26" t="s">
-        <v>397</v>
-      </c>
+      <c r="R64" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="AMH64" s="28"/>
       <c r="AMI64" s="28"/>
-      <c r="AMJ64" s="28"/>
+      <c r="AMJ64" s="0"/>
     </row>
     <row r="65" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="44" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B65" s="44" t="n">
         <v>1</v>
       </c>
       <c r="C65" s="45"/>
       <c r="D65" s="44" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E65" s="45"/>
       <c r="F65" s="46"/>
@@ -5294,25 +5209,26 @@
         <f aca="false">L65*M65</f>
         <v>330</v>
       </c>
-      <c r="P65" s="44" t="s">
-        <v>400</v>
-      </c>
-      <c r="S65" s="44" t="s">
-        <v>401</v>
-      </c>
+      <c r="O65" s="44" t="s">
+        <v>396</v>
+      </c>
+      <c r="R65" s="44" t="s">
+        <v>397</v>
+      </c>
+      <c r="AMH65" s="46"/>
       <c r="AMI65" s="46"/>
-      <c r="AMJ65" s="46"/>
+      <c r="AMJ65" s="0"/>
     </row>
     <row r="66" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="26" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B66" s="26" t="n">
         <v>1</v>
       </c>
       <c r="C66" s="27"/>
       <c r="D66" s="26" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E66" s="27"/>
       <c r="F66" s="28"/>
@@ -5332,27 +5248,28 @@
         <f aca="false">L66*M66</f>
         <v>0</v>
       </c>
-      <c r="R66" s="50"/>
-      <c r="S66" s="26" t="s">
-        <v>404</v>
-      </c>
+      <c r="Q66" s="50"/>
+      <c r="R66" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="AMC66" s="50"/>
       <c r="AMD66" s="50"/>
       <c r="AME66" s="50"/>
       <c r="AMF66" s="50"/>
-      <c r="AMG66" s="50"/>
+      <c r="AMH66" s="28"/>
       <c r="AMI66" s="28"/>
-      <c r="AMJ66" s="28"/>
+      <c r="AMJ66" s="0"/>
     </row>
     <row r="67" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="26" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B67" s="26" t="n">
         <v>1</v>
       </c>
       <c r="C67" s="27"/>
       <c r="D67" s="26" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F67" s="28"/>
       <c r="G67" s="28"/>
@@ -5373,27 +5290,28 @@
         <f aca="false">L67*M67</f>
         <v>0</v>
       </c>
-      <c r="R67" s="50"/>
-      <c r="S67" s="26" t="s">
-        <v>404</v>
-      </c>
+      <c r="Q67" s="50"/>
+      <c r="R67" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="AMC67" s="50"/>
       <c r="AMD67" s="50"/>
       <c r="AME67" s="50"/>
       <c r="AMF67" s="50"/>
-      <c r="AMG67" s="50"/>
+      <c r="AMH67" s="28"/>
       <c r="AMI67" s="28"/>
-      <c r="AMJ67" s="28"/>
+      <c r="AMJ67" s="0"/>
     </row>
     <row r="68" s="50" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="26" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B68" s="26" t="n">
         <v>1</v>
       </c>
       <c r="C68" s="27"/>
       <c r="D68" s="26" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="E68" s="27"/>
       <c r="F68" s="28"/>
@@ -5415,27 +5333,27 @@
         <v>0</v>
       </c>
       <c r="O68" s="26"/>
-      <c r="P68" s="26"/>
-      <c r="Q68" s="27"/>
-      <c r="R68" s="26"/>
-      <c r="S68" s="26" t="s">
-        <v>408</v>
-      </c>
-      <c r="T68" s="26"/>
-      <c r="AMH68" s="26"/>
+      <c r="P68" s="27"/>
+      <c r="Q68" s="26"/>
+      <c r="R68" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="S68" s="26"/>
+      <c r="AMG68" s="26"/>
+      <c r="AMH68" s="28"/>
       <c r="AMI68" s="28"/>
-      <c r="AMJ68" s="28"/>
+      <c r="AMJ68" s="0"/>
     </row>
     <row r="69" s="49" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="44" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B69" s="44" t="n">
         <v>1</v>
       </c>
       <c r="C69" s="45"/>
       <c r="D69" s="44" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E69" s="45"/>
       <c r="F69" s="46"/>
@@ -5457,16 +5375,16 @@
         <v>0</v>
       </c>
       <c r="O69" s="44"/>
-      <c r="P69" s="44"/>
-      <c r="Q69" s="45"/>
-      <c r="R69" s="44"/>
-      <c r="S69" s="44" t="s">
-        <v>411</v>
-      </c>
-      <c r="T69" s="44"/>
-      <c r="AMH69" s="44"/>
+      <c r="P69" s="45"/>
+      <c r="Q69" s="44"/>
+      <c r="R69" s="44" t="s">
+        <v>407</v>
+      </c>
+      <c r="S69" s="44"/>
+      <c r="AMG69" s="44"/>
+      <c r="AMH69" s="46"/>
       <c r="AMI69" s="46"/>
-      <c r="AMJ69" s="46"/>
+      <c r="AMJ69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K70" s="0"/>
@@ -5476,7 +5394,7 @@
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
       <c r="M72" s="7" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="N72" s="6" t="n">
         <f aca="false">SUM(N2:N71)</f>
@@ -5486,7 +5404,7 @@
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L73" s="6"/>
       <c r="M73" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="N73" s="6" t="n">
         <f aca="false">N72/$O$79</f>
@@ -5495,79 +5413,60 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B74" s="4" t="n">
         <f aca="false">SUM(B2:B73)</f>
         <v>178</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O75" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="P75" s="0" t="s">
-        <v>415</v>
-      </c>
-    </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L76" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="O76" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="P76" s="0" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O77" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="P77" s="0" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="51" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D78" s="52"/>
       <c r="E78" s="53"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="54" t="s">
-        <v>420</v>
+        <v>413</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>414</v>
       </c>
       <c r="O79" s="4" t="n">
         <v>550</v>
       </c>
       <c r="P79" s="0" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="55" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C80" s="0"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="56" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="57" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="58" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="O83" s="14"/>
       <c r="P83" s="13"/>

</xml_diff>